<commit_message>
CHF Market: modified 1M monitor 05.06.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_YCSTDBootstrapping.xlsx
@@ -58,6 +58,7 @@
     <definedName name="YieldCurve">'General Settings'!$D$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3112,9 +3113,9 @@
         <f>[1]Libor!$D$14</f>
         <v>CHFSTD#0000</v>
       </c>
-      <c r="D26" s="6" t="b">
+      <c r="D26" s="6" t="e">
         <f>_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>

</xml_diff>

<commit_message>
CHF framework with some adjustment
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15240" windowHeight="8055" tabRatio="726"/>
+    <workbookView xWindow="18330" yWindow="-15" windowWidth="18390" windowHeight="10800" tabRatio="726" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -58,7 +58,6 @@
     <definedName name="YieldCurve">'General Settings'!$D$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -628,7 +627,7 @@
     <numFmt numFmtId="177" formatCode="0.0E+00"/>
     <numFmt numFmtId="178" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,6 +761,12 @@
       <b/>
       <u/>
       <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -1279,7 +1284,7 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="210">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1730,6 +1735,12 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2095,7 +2106,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2119,7 +2130,7 @@
     <row r="1" spans="1:33" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May  5 2015 15:27:06</v>
+        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May  6 2015 11:54:37</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2484,7 +2495,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="24">
-        <v>42130.460162037038</v>
+        <v>42131.492037037038</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2610,7 +2621,7 @@
       </c>
       <c r="D14" s="21" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_CHFYCSTD#0000</v>
+        <v>_CHFYCSTD#0019</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2984,11 +2995,11 @@
       <c r="B23" s="5"/>
       <c r="C23" s="9">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>42130</v>
+        <v>42131</v>
       </c>
       <c r="D23" s="8">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>0.83739855629855786</v>
+        <v>9.6435905033565063E-3</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -3030,11 +3041,11 @@
       <c r="B24" s="5"/>
       <c r="C24" s="7">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>60395</v>
+        <v>60398</v>
       </c>
       <c r="D24" s="6">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>-8.2542728599243123E-3</v>
+        <v>-8.2084419626768292E-3</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -3113,9 +3124,9 @@
         <f>[1]Libor!$D$14</f>
         <v>CHFSTD#0000</v>
       </c>
-      <c r="D26" s="6" t="e">
+      <c r="D26" s="6" t="b">
         <f>_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -4587,7 +4598,7 @@
       <c r="B2" s="156"/>
       <c r="C2" s="156" t="str">
         <f>Deposits!E3</f>
-        <v>obj_00233#0000</v>
+        <v>obj_00235#0004</v>
       </c>
       <c r="D2" s="156" t="str">
         <f>_xll.qlRateHelperQuoteName(C2)</f>
@@ -4598,8 +4609,8 @@
         <v>-7.4999999999999997E-3</v>
       </c>
       <c r="F2" s="157"/>
-      <c r="G2" s="158" t="b">
-        <v>0</v>
+      <c r="G2" s="58" t="b">
+        <v>1</v>
       </c>
       <c r="H2" s="158">
         <v>10</v>
@@ -4609,11 +4620,11 @@
       </c>
       <c r="J2" s="159">
         <f>_xll.qlRateHelperEarliestDate($C2,Trigger)</f>
-        <v>42130</v>
+        <v>42131</v>
       </c>
       <c r="K2" s="160">
         <f>_xll.qlRateHelperLatestDate($C2,Trigger)</f>
-        <v>42131</v>
+        <v>42132</v>
       </c>
       <c r="L2" s="57"/>
     </row>
@@ -4622,7 +4633,7 @@
       <c r="B3" s="107"/>
       <c r="C3" s="107" t="str">
         <f>Deposits!E4</f>
-        <v>obj_0022c#0000</v>
+        <v>obj_00230#0004</v>
       </c>
       <c r="D3" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C3)</f>
@@ -4630,11 +4641,11 @@
       </c>
       <c r="E3" s="108">
         <f>_xll.qlRateHelperQuoteValue($C3,Trigger)</f>
-        <v>-8.0000000000000002E-3</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="F3" s="108"/>
       <c r="G3" s="58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="58">
         <v>10</v>
@@ -4644,11 +4655,11 @@
       </c>
       <c r="J3" s="109">
         <f>_xll.qlRateHelperEarliestDate($C3,Trigger)</f>
-        <v>42131</v>
+        <v>42132</v>
       </c>
       <c r="K3" s="110">
         <f>_xll.qlRateHelperLatestDate($C3,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="L3" s="57"/>
     </row>
@@ -4657,7 +4668,7 @@
       <c r="B4" s="107"/>
       <c r="C4" s="107" t="str">
         <f>Deposits!E5</f>
-        <v>obj_0023a#0000</v>
+        <v>obj_00237#0004</v>
       </c>
       <c r="D4" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C4)</f>
@@ -4679,11 +4690,11 @@
       </c>
       <c r="J4" s="109">
         <f>_xll.qlRateHelperEarliestDate($C4,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K4" s="110">
         <f>_xll.qlRateHelperLatestDate($C4,Trigger)</f>
-        <v>42135</v>
+        <v>42136</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4691,7 +4702,7 @@
       <c r="B5" s="107"/>
       <c r="C5" s="107" t="str">
         <f>Deposits!E6</f>
-        <v>obj_00236#0000</v>
+        <v>obj_00236#0004</v>
       </c>
       <c r="D5" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C5)</f>
@@ -4699,7 +4710,7 @@
       </c>
       <c r="E5" s="108">
         <f>_xll.qlRateHelperQuoteValue($C5,Trigger)</f>
-        <v>-8.0800000000000004E-3</v>
+        <v>-8.0600000000000012E-3</v>
       </c>
       <c r="F5" s="108"/>
       <c r="G5" s="58" t="b">
@@ -4713,11 +4724,11 @@
       </c>
       <c r="J5" s="109">
         <f>_xll.qlRateHelperEarliestDate($C5,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K5" s="110">
         <f>_xll.qlRateHelperLatestDate($C5,Trigger)</f>
-        <v>42139</v>
+        <v>42142</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4725,7 +4736,7 @@
       <c r="B6" s="107"/>
       <c r="C6" s="107" t="str">
         <f>Deposits!E7</f>
-        <v>obj_00234#0000</v>
+        <v>obj_00238#0004</v>
       </c>
       <c r="D6" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C6)</f>
@@ -4747,11 +4758,11 @@
       </c>
       <c r="J6" s="109">
         <f>_xll.qlRateHelperEarliestDate($C6,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K6" s="110">
         <f>_xll.qlRateHelperLatestDate($C6,Trigger)</f>
-        <v>42163</v>
+        <v>42166</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4759,7 +4770,7 @@
       <c r="B7" s="107"/>
       <c r="C7" s="107" t="str">
         <f>Deposits!E8</f>
-        <v>obj_00235#0000</v>
+        <v>obj_0023a#0004</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C7)</f>
@@ -4781,11 +4792,11 @@
       </c>
       <c r="J7" s="109">
         <f>_xll.qlRateHelperEarliestDate($C7,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K7" s="110">
         <f>_xll.qlRateHelperLatestDate($C7,Trigger)</f>
-        <v>42193</v>
+        <v>42198</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4793,7 +4804,7 @@
       <c r="B8" s="107"/>
       <c r="C8" s="107" t="str">
         <f>Deposits!E9</f>
-        <v>obj_00237#0000</v>
+        <v>obj_00239#0004</v>
       </c>
       <c r="D8" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C8)</f>
@@ -4815,11 +4826,11 @@
       </c>
       <c r="J8" s="109">
         <f>_xll.qlRateHelperEarliestDate($C8,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K8" s="110">
         <f>_xll.qlRateHelperLatestDate($C8,Trigger)</f>
-        <v>42226</v>
+        <v>42227</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4827,7 +4838,7 @@
       <c r="B9" s="107"/>
       <c r="C9" s="107" t="str">
         <f>Deposits!E10</f>
-        <v>obj_00238#0000</v>
+        <v>obj_00233#0004</v>
       </c>
       <c r="D9" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C9)</f>
@@ -4849,11 +4860,11 @@
       </c>
       <c r="J9" s="109">
         <f>_xll.qlRateHelperEarliestDate($C9,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K9" s="110">
         <f>_xll.qlRateHelperLatestDate($C9,Trigger)</f>
-        <v>42317</v>
+        <v>42319</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4861,7 +4872,7 @@
       <c r="B10" s="111"/>
       <c r="C10" s="111" t="str">
         <f>Deposits!E11</f>
-        <v>obj_00239#0000</v>
+        <v>obj_00234#0004</v>
       </c>
       <c r="D10" s="111" t="str">
         <f>_xll.qlRateHelperQuoteName(C10)</f>
@@ -4869,7 +4880,7 @@
       </c>
       <c r="E10" s="112">
         <f>_xll.qlRateHelperQuoteValue($C10,Trigger)</f>
-        <v>-5.8960000000000002E-3</v>
+        <v>-5.8659999999999997E-3</v>
       </c>
       <c r="F10" s="112"/>
       <c r="G10" s="113" t="b">
@@ -4883,11 +4894,11 @@
       </c>
       <c r="J10" s="114">
         <f>_xll.qlRateHelperEarliestDate($C10,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K10" s="115">
         <f>_xll.qlRateHelperLatestDate($C10,Trigger)</f>
-        <v>42499</v>
+        <v>42501</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4900,7 +4911,7 @@
       </c>
       <c r="C11" s="107" t="str">
         <f>Futures!H3</f>
-        <v>obj_0023b#0000</v>
+        <v>obj_00279#0000</v>
       </c>
       <c r="D11" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C11)</f>
@@ -4941,7 +4952,7 @@
       </c>
       <c r="C12" s="107" t="str">
         <f>Futures!H4</f>
-        <v>obj_00269#0000</v>
+        <v>obj_00252#0000</v>
       </c>
       <c r="D12" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C12)</f>
@@ -4949,7 +4960,7 @@
       </c>
       <c r="E12" s="116">
         <f>_xll.qlRateHelperQuoteValue($C12,Trigger)</f>
-        <v>0</v>
+        <v>100.795</v>
       </c>
       <c r="F12" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C12,Trigger)</f>
@@ -4982,7 +4993,7 @@
       </c>
       <c r="C13" s="107" t="str">
         <f>Futures!H5</f>
-        <v>obj_0026a#0000</v>
+        <v>obj_0024f#0000</v>
       </c>
       <c r="D13" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C13)</f>
@@ -5023,7 +5034,7 @@
       </c>
       <c r="C14" s="107" t="str">
         <f>Futures!H6</f>
-        <v>obj_00248#0000</v>
+        <v>obj_00288#0000</v>
       </c>
       <c r="D14" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C14)</f>
@@ -5064,7 +5075,7 @@
       </c>
       <c r="C15" s="107" t="str">
         <f>Futures!H7</f>
-        <v>obj_00287#0000</v>
+        <v>obj_0026e#0000</v>
       </c>
       <c r="D15" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C15)</f>
@@ -5072,7 +5083,7 @@
       </c>
       <c r="E15" s="116">
         <f>_xll.qlRateHelperQuoteValue($C15,Trigger)</f>
-        <v>0</v>
+        <v>100.785</v>
       </c>
       <c r="F15" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C15,Trigger)</f>
@@ -5105,7 +5116,7 @@
       </c>
       <c r="C16" s="107" t="str">
         <f>Futures!H8</f>
-        <v>obj_00243#0000</v>
+        <v>obj_00276#0000</v>
       </c>
       <c r="D16" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C16)</f>
@@ -5146,7 +5157,7 @@
       </c>
       <c r="C17" s="107" t="str">
         <f>Futures!H9</f>
-        <v>obj_00260#0000</v>
+        <v>obj_00263#0000</v>
       </c>
       <c r="D17" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C17)</f>
@@ -5187,7 +5198,7 @@
       </c>
       <c r="C18" s="107" t="str">
         <f>Futures!H10</f>
-        <v>obj_0026d#0000</v>
+        <v>obj_0023b#0000</v>
       </c>
       <c r="D18" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C18)</f>
@@ -5195,7 +5206,7 @@
       </c>
       <c r="E18" s="116">
         <f>_xll.qlRateHelperQuoteValue($C18,Trigger)</f>
-        <v>0</v>
+        <v>100.745</v>
       </c>
       <c r="F18" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C18,Trigger)</f>
@@ -5228,7 +5239,7 @@
       </c>
       <c r="C19" s="107" t="str">
         <f>Futures!H11</f>
-        <v>obj_00259#0000</v>
+        <v>obj_00242#0000</v>
       </c>
       <c r="D19" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C19)</f>
@@ -5269,7 +5280,7 @@
       </c>
       <c r="C20" s="107" t="str">
         <f>Futures!H12</f>
-        <v>obj_00245#0000</v>
+        <v>obj_0025e#0000</v>
       </c>
       <c r="D20" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C20)</f>
@@ -5310,7 +5321,7 @@
       </c>
       <c r="C21" s="107" t="str">
         <f>Futures!H13</f>
-        <v>obj_00289#0000</v>
+        <v>obj_0025a#0000</v>
       </c>
       <c r="D21" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C21)</f>
@@ -5318,7 +5329,7 @@
       </c>
       <c r="E21" s="116">
         <f>_xll.qlRateHelperQuoteValue($C21,Trigger)</f>
-        <v>0</v>
+        <v>100.67500000000001</v>
       </c>
       <c r="F21" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C21,Trigger)</f>
@@ -5351,7 +5362,7 @@
       </c>
       <c r="C22" s="107" t="str">
         <f>Futures!H14</f>
-        <v>obj_0027e#0000</v>
+        <v>obj_00265#0000</v>
       </c>
       <c r="D22" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C22)</f>
@@ -5392,7 +5403,7 @@
       </c>
       <c r="C23" s="107" t="str">
         <f>Futures!H15</f>
-        <v>obj_0025f#0000</v>
+        <v>obj_0026d#0000</v>
       </c>
       <c r="D23" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C23)</f>
@@ -5400,7 +5411,7 @@
       </c>
       <c r="E23" s="116">
         <f>_xll.qlRateHelperQuoteValue($C23,Trigger)</f>
-        <v>0</v>
+        <v>100.605</v>
       </c>
       <c r="F23" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C23,Trigger)</f>
@@ -5433,7 +5444,7 @@
       </c>
       <c r="C24" s="107" t="str">
         <f>Futures!H16</f>
-        <v>obj_00247#0000</v>
+        <v>obj_0026a#0000</v>
       </c>
       <c r="D24" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C24)</f>
@@ -5441,7 +5452,7 @@
       </c>
       <c r="E24" s="116">
         <f>_xll.qlRateHelperQuoteValue($C24,Trigger)</f>
-        <v>0</v>
+        <v>100.545</v>
       </c>
       <c r="F24" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C24,Trigger)</f>
@@ -5474,7 +5485,7 @@
       </c>
       <c r="C25" s="107" t="str">
         <f>Futures!H17</f>
-        <v>obj_00249#0000</v>
+        <v>obj_0023f#0000</v>
       </c>
       <c r="D25" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C25)</f>
@@ -5482,7 +5493,7 @@
       </c>
       <c r="E25" s="116">
         <f>_xll.qlRateHelperQuoteValue($C25,Trigger)</f>
-        <v>0</v>
+        <v>100.47499999999999</v>
       </c>
       <c r="F25" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C25,Trigger)</f>
@@ -5515,7 +5526,7 @@
       </c>
       <c r="C26" s="107" t="str">
         <f>Futures!H18</f>
-        <v>obj_0027d#0000</v>
+        <v>obj_00281#0000</v>
       </c>
       <c r="D26" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C26)</f>
@@ -5523,7 +5534,7 @@
       </c>
       <c r="E26" s="116">
         <f>_xll.qlRateHelperQuoteValue($C26,Trigger)</f>
-        <v>0</v>
+        <v>100.405</v>
       </c>
       <c r="F26" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C26,Trigger)</f>
@@ -5556,7 +5567,7 @@
       </c>
       <c r="C27" s="107" t="str">
         <f>Futures!H19</f>
-        <v>obj_00278#0000</v>
+        <v>obj_0024a#0000</v>
       </c>
       <c r="D27" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C27)</f>
@@ -5564,7 +5575,7 @@
       </c>
       <c r="E27" s="116">
         <f>_xll.qlRateHelperQuoteValue($C27,Trigger)</f>
-        <v>0</v>
+        <v>100.32</v>
       </c>
       <c r="F27" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C27,Trigger)</f>
@@ -5597,7 +5608,7 @@
       </c>
       <c r="C28" s="107" t="str">
         <f>Futures!H20</f>
-        <v>obj_00283#0000</v>
+        <v>obj_00277#0000</v>
       </c>
       <c r="D28" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C28)</f>
@@ -5605,7 +5616,7 @@
       </c>
       <c r="E28" s="116">
         <f>_xll.qlRateHelperQuoteValue($C28,Trigger)</f>
-        <v>0</v>
+        <v>100.23500000000001</v>
       </c>
       <c r="F28" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C28,Trigger)</f>
@@ -5638,7 +5649,7 @@
       </c>
       <c r="C29" s="107" t="str">
         <f>Futures!H21</f>
-        <v>obj_00254#0000</v>
+        <v>obj_00262#0000</v>
       </c>
       <c r="D29" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C29)</f>
@@ -5646,7 +5657,7 @@
       </c>
       <c r="E29" s="116">
         <f>_xll.qlRateHelperQuoteValue($C29,Trigger)</f>
-        <v>0</v>
+        <v>100.14000000000001</v>
       </c>
       <c r="F29" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C29,Trigger)</f>
@@ -5679,7 +5690,7 @@
       </c>
       <c r="C30" s="107" t="str">
         <f>Futures!H22</f>
-        <v>obj_0025e#0000</v>
+        <v>obj_00267#0000</v>
       </c>
       <c r="D30" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C30)</f>
@@ -5687,7 +5698,7 @@
       </c>
       <c r="E30" s="116">
         <f>_xll.qlRateHelperQuoteValue($C30,Trigger)</f>
-        <v>0</v>
+        <v>100.04500000000002</v>
       </c>
       <c r="F30" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C30,Trigger)</f>
@@ -5720,7 +5731,7 @@
       </c>
       <c r="C31" s="107" t="str">
         <f>Futures!H23</f>
-        <v>obj_0026e#0000</v>
+        <v>obj_00259#0000</v>
       </c>
       <c r="D31" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C31)</f>
@@ -5728,7 +5739,7 @@
       </c>
       <c r="E31" s="116">
         <f>_xll.qlRateHelperQuoteValue($C31,Trigger)</f>
-        <v>0</v>
+        <v>99.93</v>
       </c>
       <c r="F31" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C31,Trigger)</f>
@@ -5761,7 +5772,7 @@
       </c>
       <c r="C32" s="107" t="str">
         <f>Futures!H24</f>
-        <v>obj_00240#0000</v>
+        <v>obj_00250#0000</v>
       </c>
       <c r="D32" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C32)</f>
@@ -5769,7 +5780,7 @@
       </c>
       <c r="E32" s="116">
         <f>_xll.qlRateHelperQuoteValue($C32,Trigger)</f>
-        <v>0</v>
+        <v>49.97</v>
       </c>
       <c r="F32" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C32,Trigger)</f>
@@ -5802,7 +5813,7 @@
       </c>
       <c r="C33" s="107" t="str">
         <f>Futures!H25</f>
-        <v>obj_00257#0000</v>
+        <v>obj_00246#0000</v>
       </c>
       <c r="D33" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C33)</f>
@@ -5810,7 +5821,7 @@
       </c>
       <c r="E33" s="116">
         <f>_xll.qlRateHelperQuoteValue($C33,Trigger)</f>
-        <v>0</v>
+        <v>49.965000000000003</v>
       </c>
       <c r="F33" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C33,Trigger)</f>
@@ -5843,7 +5854,7 @@
       </c>
       <c r="C34" s="107" t="str">
         <f>Futures!H26</f>
-        <v>obj_0024a#0000</v>
+        <v>obj_0027a#0000</v>
       </c>
       <c r="D34" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C34)</f>
@@ -5851,7 +5862,7 @@
       </c>
       <c r="E34" s="116">
         <f>_xll.qlRateHelperQuoteValue($C34,Trigger)</f>
-        <v>0</v>
+        <v>49.965000000000003</v>
       </c>
       <c r="F34" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C34,Trigger)</f>
@@ -5884,7 +5895,7 @@
       </c>
       <c r="C35" s="107" t="str">
         <f>Futures!H27</f>
-        <v>obj_00279#0000</v>
+        <v>obj_0026c#0000</v>
       </c>
       <c r="D35" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C35)</f>
@@ -5892,7 +5903,7 @@
       </c>
       <c r="E35" s="116">
         <f>_xll.qlRateHelperQuoteValue($C35,Trigger)</f>
-        <v>0</v>
+        <v>49.97</v>
       </c>
       <c r="F35" s="108">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($C35,Trigger)</f>
@@ -5925,7 +5936,7 @@
       </c>
       <c r="C36" s="107" t="str">
         <f>Futures!H28</f>
-        <v>obj_00273#0000</v>
+        <v>obj_0023e#0000</v>
       </c>
       <c r="D36" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C36)</f>
@@ -5966,7 +5977,7 @@
       </c>
       <c r="C37" s="107" t="str">
         <f>Futures!H29</f>
-        <v>obj_0025c#0000</v>
+        <v>obj_00271#0000</v>
       </c>
       <c r="D37" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C37)</f>
@@ -6007,7 +6018,7 @@
       </c>
       <c r="C38" s="107" t="str">
         <f>Futures!H30</f>
-        <v>obj_00251#0000</v>
+        <v>obj_0025b#0000</v>
       </c>
       <c r="D38" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C38)</f>
@@ -6048,7 +6059,7 @@
       </c>
       <c r="C39" s="107" t="str">
         <f>Futures!H31</f>
-        <v>obj_00271#0000</v>
+        <v>obj_00256#0000</v>
       </c>
       <c r="D39" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C39)</f>
@@ -6089,7 +6100,7 @@
       </c>
       <c r="C40" s="107" t="str">
         <f>Futures!H32</f>
-        <v>obj_00262#0000</v>
+        <v>obj_00269#0000</v>
       </c>
       <c r="D40" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C40)</f>
@@ -6130,7 +6141,7 @@
       </c>
       <c r="C41" s="107" t="str">
         <f>Futures!H33</f>
-        <v>obj_0024e#0000</v>
+        <v>obj_00258#0000</v>
       </c>
       <c r="D41" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C41)</f>
@@ -6171,7 +6182,7 @@
       </c>
       <c r="C42" s="107" t="str">
         <f>Futures!H34</f>
-        <v>obj_0023e#0000</v>
+        <v>obj_00286#0000</v>
       </c>
       <c r="D42" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C42)</f>
@@ -6212,7 +6223,7 @@
       </c>
       <c r="C43" s="107" t="str">
         <f>Futures!H35</f>
-        <v>obj_0023c#0000</v>
+        <v>obj_00249#0000</v>
       </c>
       <c r="D43" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C43)</f>
@@ -6253,7 +6264,7 @@
       </c>
       <c r="C44" s="107" t="str">
         <f>Futures!H36</f>
-        <v>obj_00272#0000</v>
+        <v>obj_0026f#0000</v>
       </c>
       <c r="D44" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C44)</f>
@@ -6294,7 +6305,7 @@
       </c>
       <c r="C45" s="107" t="str">
         <f>Futures!H37</f>
-        <v>obj_00266#0000</v>
+        <v>obj_0026b#0000</v>
       </c>
       <c r="D45" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C45)</f>
@@ -6335,7 +6346,7 @@
       </c>
       <c r="C46" s="107" t="str">
         <f>Futures!H38</f>
-        <v>obj_0024d#0000</v>
+        <v>obj_00255#0000</v>
       </c>
       <c r="D46" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C46)</f>
@@ -6376,7 +6387,7 @@
       </c>
       <c r="C47" s="107" t="str">
         <f>Futures!H39</f>
-        <v>obj_00270#0000</v>
+        <v>obj_00241#0000</v>
       </c>
       <c r="D47" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C47)</f>
@@ -6417,7 +6428,7 @@
       </c>
       <c r="C48" s="107" t="str">
         <f>Futures!H40</f>
-        <v>obj_0025a#0000</v>
+        <v>obj_0024c#0000</v>
       </c>
       <c r="D48" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C48)</f>
@@ -6458,7 +6469,7 @@
       </c>
       <c r="C49" s="107" t="str">
         <f>Futures!H41</f>
-        <v>obj_00267#0000</v>
+        <v>obj_0027d#0000</v>
       </c>
       <c r="D49" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C49)</f>
@@ -6499,7 +6510,7 @@
       </c>
       <c r="C50" s="107" t="str">
         <f>Futures!H42</f>
-        <v>obj_00246#0000</v>
+        <v>obj_00253#0000</v>
       </c>
       <c r="D50" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C50)</f>
@@ -6540,7 +6551,7 @@
       </c>
       <c r="C51" s="107" t="str">
         <f>Futures!H43</f>
-        <v>obj_00281#0000</v>
+        <v>obj_0025c#0000</v>
       </c>
       <c r="D51" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C51)</f>
@@ -6581,7 +6592,7 @@
       </c>
       <c r="C52" s="111" t="str">
         <f>Futures!H44</f>
-        <v>obj_00244#0000</v>
+        <v>obj_0023d#0000</v>
       </c>
       <c r="D52" s="111" t="str">
         <f>_xll.qlRateHelperQuoteName(C52)</f>
@@ -6633,7 +6644,7 @@
         <f>_xll.qlSwapRateHelperSpread($C53,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="158" t="b">
+      <c r="G53" s="210" t="b">
         <v>0</v>
       </c>
       <c r="H53" s="158">
@@ -6644,11 +6655,11 @@
       </c>
       <c r="J53" s="159">
         <f>_xll.qlRateHelperEarliestDate($C53,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K53" s="160">
         <f>_xll.qlRateHelperLatestDate($C53,Trigger)</f>
-        <v>42317</v>
+        <v>42319</v>
       </c>
       <c r="M53" s="119"/>
     </row>
@@ -6657,7 +6668,7 @@
       <c r="B54" s="107"/>
       <c r="C54" s="107" t="str">
         <f>Swaps!K6</f>
-        <v>obj_00241#0000</v>
+        <v>obj_00261#0000</v>
       </c>
       <c r="D54" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C54)</f>
@@ -6665,13 +6676,13 @@
       </c>
       <c r="E54" s="108">
         <f>_xll.qlRateHelperQuoteValue($C54,Trigger)</f>
-        <v>-7.1999999999999998E-3</v>
+        <v>-6.8000000000000005E-3</v>
       </c>
       <c r="F54" s="108">
         <f>_xll.qlSwapRateHelperSpread($C54,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="58" t="b">
+      <c r="G54" s="211" t="b">
         <v>0</v>
       </c>
       <c r="H54" s="58">
@@ -6682,11 +6693,11 @@
       </c>
       <c r="J54" s="109">
         <f>_xll.qlRateHelperEarliestDate($C54,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K54" s="110">
         <f>_xll.qlRateHelperLatestDate($C54,Trigger)</f>
-        <v>42499</v>
+        <v>42501</v>
       </c>
       <c r="M54" s="119"/>
     </row>
@@ -6695,7 +6706,7 @@
       <c r="B55" s="107"/>
       <c r="C55" s="107" t="str">
         <f>Swaps!K7</f>
-        <v>obj_00284#0000</v>
+        <v>obj_00254#0000</v>
       </c>
       <c r="D55" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C55)</f>
@@ -6709,7 +6720,7 @@
         <f>_xll.qlSwapRateHelperSpread($C55,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="58" t="b">
+      <c r="G55" s="211" t="b">
         <v>0</v>
       </c>
       <c r="H55" s="58">
@@ -6720,11 +6731,11 @@
       </c>
       <c r="J55" s="109">
         <f>_xll.qlRateHelperEarliestDate($C55,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K55" s="110">
         <f>_xll.qlRateHelperLatestDate($C55,Trigger)</f>
-        <v>42590</v>
+        <v>42593</v>
       </c>
       <c r="M55" s="119"/>
     </row>
@@ -6733,7 +6744,7 @@
       <c r="B56" s="107"/>
       <c r="C56" s="107" t="str">
         <f>Swaps!K8</f>
-        <v>obj_00255#0000</v>
+        <v>obj_00257#0000</v>
       </c>
       <c r="D56" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C56)</f>
@@ -6747,7 +6758,7 @@
         <f>_xll.qlSwapRateHelperSpread($C56,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="G56" s="58" t="b">
+      <c r="G56" s="211" t="b">
         <v>0</v>
       </c>
       <c r="H56" s="58">
@@ -6758,11 +6769,11 @@
       </c>
       <c r="J56" s="109">
         <f>_xll.qlRateHelperEarliestDate($C56,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K56" s="110">
         <f>_xll.qlRateHelperLatestDate($C56,Trigger)</f>
-        <v>42682</v>
+        <v>42685</v>
       </c>
       <c r="M56" s="119"/>
     </row>
@@ -6771,7 +6782,7 @@
       <c r="B57" s="107"/>
       <c r="C57" s="107" t="str">
         <f>Swaps!K9</f>
-        <v>obj_0027c#0000</v>
+        <v>obj_0024e#0000</v>
       </c>
       <c r="D57" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C57)</f>
@@ -6785,7 +6796,7 @@
         <f>_xll.qlSwapRateHelperSpread($C57,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="58" t="b">
+      <c r="G57" s="211" t="b">
         <v>0</v>
       </c>
       <c r="H57" s="58">
@@ -6796,11 +6807,11 @@
       </c>
       <c r="J57" s="109">
         <f>_xll.qlRateHelperEarliestDate($C57,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K57" s="110">
         <f>_xll.qlRateHelperLatestDate($C57,Trigger)</f>
-        <v>42774</v>
+        <v>42779</v>
       </c>
       <c r="M57" s="119"/>
     </row>
@@ -6809,7 +6820,7 @@
       <c r="B58" s="107"/>
       <c r="C58" s="107" t="str">
         <f>Swaps!K10</f>
-        <v>obj_0024c#0000</v>
+        <v>obj_00264#0000</v>
       </c>
       <c r="D58" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C58)</f>
@@ -6817,7 +6828,7 @@
       </c>
       <c r="E58" s="108">
         <f>_xll.qlRateHelperQuoteValue($C58,Trigger)</f>
-        <v>-6.4000000000000003E-3</v>
+        <v>-5.6000000000000008E-3</v>
       </c>
       <c r="F58" s="108">
         <f>_xll.qlSwapRateHelperSpread($C58,Trigger)</f>
@@ -6835,11 +6846,11 @@
       </c>
       <c r="J58" s="109">
         <f>_xll.qlRateHelperEarliestDate($C58,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K58" s="110">
         <f>_xll.qlRateHelperLatestDate($C58,Trigger)</f>
-        <v>42863</v>
+        <v>42866</v>
       </c>
       <c r="M58" s="119"/>
       <c r="O58" s="162"/>
@@ -6849,7 +6860,7 @@
       <c r="B59" s="107"/>
       <c r="C59" s="107" t="str">
         <f>Swaps!K11</f>
-        <v>obj_0026c#0000</v>
+        <v>obj_00273#0000</v>
       </c>
       <c r="D59" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C59)</f>
@@ -6857,7 +6868,7 @@
       </c>
       <c r="E59" s="108">
         <f>_xll.qlRateHelperQuoteValue($C59,Trigger)</f>
-        <v>-5.1999999999999998E-3</v>
+        <v>-4.2000000000000006E-3</v>
       </c>
       <c r="F59" s="108">
         <f>_xll.qlSwapRateHelperSpread($C59,Trigger)</f>
@@ -6875,11 +6886,11 @@
       </c>
       <c r="J59" s="109">
         <f>_xll.qlRateHelperEarliestDate($C59,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K59" s="110">
         <f>_xll.qlRateHelperLatestDate($C59,Trigger)</f>
-        <v>43228</v>
+        <v>43231</v>
       </c>
       <c r="M59" s="119"/>
       <c r="O59" s="162"/>
@@ -6889,7 +6900,7 @@
       <c r="B60" s="107"/>
       <c r="C60" s="107" t="str">
         <f>Swaps!K12</f>
-        <v>obj_00275#0000</v>
+        <v>obj_00245#0000</v>
       </c>
       <c r="D60" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C60)</f>
@@ -6897,7 +6908,7 @@
       </c>
       <c r="E60" s="108">
         <f>_xll.qlRateHelperQuoteValue($C60,Trigger)</f>
-        <v>-3.7499999999999999E-3</v>
+        <v>-2.575E-3</v>
       </c>
       <c r="F60" s="108">
         <f>_xll.qlSwapRateHelperSpread($C60,Trigger)</f>
@@ -6915,11 +6926,11 @@
       </c>
       <c r="J60" s="109">
         <f>_xll.qlRateHelperEarliestDate($C60,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K60" s="110">
         <f>_xll.qlRateHelperLatestDate($C60,Trigger)</f>
-        <v>43593</v>
+        <v>43598</v>
       </c>
       <c r="M60" s="119"/>
       <c r="O60" s="162"/>
@@ -6929,7 +6940,7 @@
       <c r="B61" s="107"/>
       <c r="C61" s="107" t="str">
         <f>Swaps!K13</f>
-        <v>obj_00265#0000</v>
+        <v>obj_00284#0000</v>
       </c>
       <c r="D61" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C61)</f>
@@ -6937,7 +6948,7 @@
       </c>
       <c r="E61" s="108">
         <f>_xll.qlRateHelperQuoteValue($C61,Trigger)</f>
-        <v>-2.2750000000000001E-3</v>
+        <v>-8.5000000000000006E-4</v>
       </c>
       <c r="F61" s="108">
         <f>_xll.qlSwapRateHelperSpread($C61,Trigger)</f>
@@ -6955,11 +6966,11 @@
       </c>
       <c r="J61" s="109">
         <f>_xll.qlRateHelperEarliestDate($C61,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K61" s="110">
         <f>_xll.qlRateHelperLatestDate($C61,Trigger)</f>
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="M61" s="119"/>
       <c r="O61" s="162"/>
@@ -6969,7 +6980,7 @@
       <c r="B62" s="107"/>
       <c r="C62" s="107" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00277#0000</v>
+        <v>obj_00282#0000</v>
       </c>
       <c r="D62" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C62)</f>
@@ -6977,7 +6988,7 @@
       </c>
       <c r="E62" s="108">
         <f>_xll.qlRateHelperQuoteValue($C62,Trigger)</f>
-        <v>-8.7499999999999991E-4</v>
+        <v>7.2500000000000006E-4</v>
       </c>
       <c r="F62" s="108">
         <f>_xll.qlSwapRateHelperSpread($C62,Trigger)</f>
@@ -6995,11 +7006,11 @@
       </c>
       <c r="J62" s="109">
         <f>_xll.qlRateHelperEarliestDate($C62,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K62" s="110">
         <f>_xll.qlRateHelperLatestDate($C62,Trigger)</f>
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="M62" s="119"/>
       <c r="O62" s="162"/>
@@ -7009,7 +7020,7 @@
       <c r="B63" s="107"/>
       <c r="C63" s="107" t="str">
         <f>Swaps!K15</f>
-        <v>obj_00250#0000</v>
+        <v>obj_00248#0000</v>
       </c>
       <c r="D63" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C63)</f>
@@ -7017,7 +7028,7 @@
       </c>
       <c r="E63" s="108">
         <f>_xll.qlRateHelperQuoteValue($C63,Trigger)</f>
-        <v>3.4999999999999994E-4</v>
+        <v>2.1000000000000003E-3</v>
       </c>
       <c r="F63" s="108">
         <f>_xll.qlSwapRateHelperSpread($C63,Trigger)</f>
@@ -7035,11 +7046,11 @@
       </c>
       <c r="J63" s="109">
         <f>_xll.qlRateHelperEarliestDate($C63,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K63" s="110">
         <f>_xll.qlRateHelperLatestDate($C63,Trigger)</f>
-        <v>44690</v>
+        <v>44692</v>
       </c>
       <c r="M63" s="119"/>
       <c r="O63" s="162"/>
@@ -7049,7 +7060,7 @@
       <c r="B64" s="107"/>
       <c r="C64" s="107" t="str">
         <f>Swaps!K16</f>
-        <v>obj_0027b#0000</v>
+        <v>obj_00274#0000</v>
       </c>
       <c r="D64" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C64)</f>
@@ -7057,7 +7068,7 @@
       </c>
       <c r="E64" s="108">
         <f>_xll.qlRateHelperQuoteValue($C64,Trigger)</f>
-        <v>1.4000000000000002E-3</v>
+        <v>3.2750000000000001E-3</v>
       </c>
       <c r="F64" s="108">
         <f>_xll.qlSwapRateHelperSpread($C64,Trigger)</f>
@@ -7075,11 +7086,11 @@
       </c>
       <c r="J64" s="109">
         <f>_xll.qlRateHelperEarliestDate($C64,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K64" s="110">
         <f>_xll.qlRateHelperLatestDate($C64,Trigger)</f>
-        <v>45054</v>
+        <v>45057</v>
       </c>
       <c r="M64" s="119"/>
       <c r="O64" s="162"/>
@@ -7089,7 +7100,7 @@
       <c r="B65" s="107"/>
       <c r="C65" s="107" t="str">
         <f>Swaps!K17</f>
-        <v>obj_00256#0000</v>
+        <v>obj_0025d#0000</v>
       </c>
       <c r="D65" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C65)</f>
@@ -7097,7 +7108,7 @@
       </c>
       <c r="E65" s="108">
         <f>_xll.qlRateHelperQuoteValue($C65,Trigger)</f>
-        <v>2.2750000000000001E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
       <c r="F65" s="108">
         <f>_xll.qlSwapRateHelperSpread($C65,Trigger)</f>
@@ -7115,11 +7126,11 @@
       </c>
       <c r="J65" s="109">
         <f>_xll.qlRateHelperEarliestDate($C65,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K65" s="110">
         <f>_xll.qlRateHelperLatestDate($C65,Trigger)</f>
-        <v>45420</v>
+        <v>45425</v>
       </c>
       <c r="M65" s="119"/>
       <c r="O65" s="162"/>
@@ -7129,7 +7140,7 @@
       <c r="B66" s="107"/>
       <c r="C66" s="107" t="str">
         <f>Swaps!K18</f>
-        <v>obj_0023d#0000</v>
+        <v>obj_00272#0000</v>
       </c>
       <c r="D66" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C66)</f>
@@ -7137,7 +7148,7 @@
       </c>
       <c r="E66" s="108">
         <f>_xll.qlRateHelperQuoteValue($C66,Trigger)</f>
-        <v>3.0000000000000005E-3</v>
+        <v>5.0499999999999998E-3</v>
       </c>
       <c r="F66" s="108">
         <f>_xll.qlSwapRateHelperSpread($C66,Trigger)</f>
@@ -7155,11 +7166,11 @@
       </c>
       <c r="J66" s="109">
         <f>_xll.qlRateHelperEarliestDate($C66,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K66" s="110">
         <f>_xll.qlRateHelperLatestDate($C66,Trigger)</f>
-        <v>45785</v>
+        <v>45789</v>
       </c>
       <c r="M66" s="119"/>
       <c r="O66" s="162"/>
@@ -7169,7 +7180,7 @@
       <c r="B67" s="107"/>
       <c r="C67" s="107" t="str">
         <f>Swaps!K19</f>
-        <v>obj_00242#0000</v>
+        <v>obj_00251#0000</v>
       </c>
       <c r="D67" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C67)</f>
@@ -7177,7 +7188,7 @@
       </c>
       <c r="E67" s="108">
         <f>_xll.qlRateHelperQuoteValue($C67,Trigger)</f>
-        <v>3.5750000000000005E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="F67" s="108">
         <f>_xll.qlSwapRateHelperSpread($C67,Trigger)</f>
@@ -7195,11 +7206,11 @@
       </c>
       <c r="J67" s="109">
         <f>_xll.qlRateHelperEarliestDate($C67,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K67" s="110">
         <f>_xll.qlRateHelperLatestDate($C67,Trigger)</f>
-        <v>46150</v>
+        <v>46153</v>
       </c>
       <c r="M67" s="119"/>
       <c r="O67" s="162"/>
@@ -7209,7 +7220,7 @@
       <c r="B68" s="107"/>
       <c r="C68" s="107" t="str">
         <f>Swaps!K20</f>
-        <v>obj_00282#0000</v>
+        <v>obj_0024d#0000</v>
       </c>
       <c r="D68" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C68)</f>
@@ -7217,7 +7228,7 @@
       </c>
       <c r="E68" s="108">
         <f>_xll.qlRateHelperQuoteValue($C68,Trigger)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="F68" s="108">
         <f>_xll.qlSwapRateHelperSpread($C68,Trigger)</f>
@@ -7235,11 +7246,11 @@
       </c>
       <c r="J68" s="109">
         <f>_xll.qlRateHelperEarliestDate($C68,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K68" s="110">
         <f>_xll.qlRateHelperLatestDate($C68,Trigger)</f>
-        <v>46517</v>
+        <v>46518</v>
       </c>
       <c r="M68" s="119"/>
       <c r="O68" s="162"/>
@@ -7249,7 +7260,7 @@
       <c r="B69" s="107"/>
       <c r="C69" s="107" t="str">
         <f>Swaps!K21</f>
-        <v>obj_0026b#0000</v>
+        <v>obj_00244#0000</v>
       </c>
       <c r="D69" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C69)</f>
@@ -7275,11 +7286,11 @@
       </c>
       <c r="J69" s="109">
         <f>_xll.qlRateHelperEarliestDate($C69,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K69" s="110">
         <f>_xll.qlRateHelperLatestDate($C69,Trigger)</f>
-        <v>46881</v>
+        <v>46884</v>
       </c>
       <c r="M69" s="119"/>
       <c r="O69" s="162"/>
@@ -7289,7 +7300,7 @@
       <c r="B70" s="107"/>
       <c r="C70" s="107" t="str">
         <f>Swaps!K22</f>
-        <v>obj_0023f#0000</v>
+        <v>obj_00280#0000</v>
       </c>
       <c r="D70" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C70)</f>
@@ -7315,11 +7326,11 @@
       </c>
       <c r="J70" s="109">
         <f>_xll.qlRateHelperEarliestDate($C70,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K70" s="110">
         <f>_xll.qlRateHelperLatestDate($C70,Trigger)</f>
-        <v>47246</v>
+        <v>47249</v>
       </c>
       <c r="M70" s="119"/>
       <c r="O70" s="162"/>
@@ -7329,7 +7340,7 @@
       <c r="B71" s="107"/>
       <c r="C71" s="107" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00285#0000</v>
+        <v>obj_0027b#0000</v>
       </c>
       <c r="D71" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C71)</f>
@@ -7337,7 +7348,7 @@
       </c>
       <c r="E71" s="108">
         <f>_xll.qlRateHelperQuoteValue($C71,Trigger)</f>
-        <v>5.3E-3</v>
+        <v>7.575000000000001E-3</v>
       </c>
       <c r="F71" s="108">
         <f>_xll.qlSwapRateHelperSpread($C71,Trigger)</f>
@@ -7355,11 +7366,11 @@
       </c>
       <c r="J71" s="109">
         <f>_xll.qlRateHelperEarliestDate($C71,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K71" s="110">
         <f>_xll.qlRateHelperLatestDate($C71,Trigger)</f>
-        <v>47611</v>
+        <v>47616</v>
       </c>
       <c r="M71" s="119"/>
       <c r="O71" s="162"/>
@@ -7369,7 +7380,7 @@
       <c r="B72" s="107"/>
       <c r="C72" s="107" t="str">
         <f>Swaps!K24</f>
-        <v>obj_0024f#0000</v>
+        <v>obj_0023c#0000</v>
       </c>
       <c r="D72" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C72)</f>
@@ -7395,11 +7406,11 @@
       </c>
       <c r="J72" s="109">
         <f>_xll.qlRateHelperEarliestDate($C72,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K72" s="110">
         <f>_xll.qlRateHelperLatestDate($C72,Trigger)</f>
-        <v>47976</v>
+        <v>47980</v>
       </c>
       <c r="M72" s="119"/>
       <c r="O72" s="162"/>
@@ -7409,7 +7420,7 @@
       <c r="B73" s="107"/>
       <c r="C73" s="107" t="str">
         <f>Swaps!K25</f>
-        <v>obj_00261#0000</v>
+        <v>obj_0024b#0000</v>
       </c>
       <c r="D73" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C73)</f>
@@ -7435,11 +7446,11 @@
       </c>
       <c r="J73" s="109">
         <f>_xll.qlRateHelperEarliestDate($C73,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K73" s="110">
         <f>_xll.qlRateHelperLatestDate($C73,Trigger)</f>
-        <v>48344</v>
+        <v>48345</v>
       </c>
       <c r="M73" s="119"/>
       <c r="O73" s="162"/>
@@ -7449,7 +7460,7 @@
       <c r="B74" s="107"/>
       <c r="C74" s="107" t="str">
         <f>Swaps!K26</f>
-        <v>obj_0026f#0000</v>
+        <v>obj_0025f#0000</v>
       </c>
       <c r="D74" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C74)</f>
@@ -7475,11 +7486,11 @@
       </c>
       <c r="J74" s="109">
         <f>_xll.qlRateHelperEarliestDate($C74,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K74" s="110">
         <f>_xll.qlRateHelperLatestDate($C74,Trigger)</f>
-        <v>48708</v>
+        <v>48710</v>
       </c>
       <c r="M74" s="119"/>
       <c r="O74" s="162"/>
@@ -7489,7 +7500,7 @@
       <c r="B75" s="107"/>
       <c r="C75" s="107" t="str">
         <f>Swaps!K27</f>
-        <v>obj_00288#0000</v>
+        <v>obj_00283#0000</v>
       </c>
       <c r="D75" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C75)</f>
@@ -7515,11 +7526,11 @@
       </c>
       <c r="J75" s="109">
         <f>_xll.qlRateHelperEarliestDate($C75,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K75" s="110">
         <f>_xll.qlRateHelperLatestDate($C75,Trigger)</f>
-        <v>49072</v>
+        <v>49075</v>
       </c>
       <c r="M75" s="119"/>
       <c r="O75" s="162"/>
@@ -7529,7 +7540,7 @@
       <c r="B76" s="107"/>
       <c r="C76" s="107" t="str">
         <f>Swaps!K28</f>
-        <v>obj_00253#0000</v>
+        <v>obj_00266#0000</v>
       </c>
       <c r="D76" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C76)</f>
@@ -7537,7 +7548,7 @@
       </c>
       <c r="E76" s="108">
         <f>_xll.qlRateHelperQuoteValue($C76,Trigger)</f>
-        <v>6.5000000000000006E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F76" s="108">
         <f>_xll.qlSwapRateHelperSpread($C76,Trigger)</f>
@@ -7555,11 +7566,11 @@
       </c>
       <c r="J76" s="109">
         <f>_xll.qlRateHelperEarliestDate($C76,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K76" s="110">
         <f>_xll.qlRateHelperLatestDate($C76,Trigger)</f>
-        <v>49437</v>
+        <v>49440</v>
       </c>
       <c r="M76" s="119"/>
       <c r="O76" s="162"/>
@@ -7569,7 +7580,7 @@
       <c r="B77" s="107"/>
       <c r="C77" s="107" t="str">
         <f>Swaps!K29</f>
-        <v>obj_00274#0000</v>
+        <v>obj_00275#0000</v>
       </c>
       <c r="D77" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C77)</f>
@@ -7595,11 +7606,11 @@
       </c>
       <c r="J77" s="109">
         <f>_xll.qlRateHelperEarliestDate($C77,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K77" s="110">
         <f>_xll.qlRateHelperLatestDate($C77,Trigger)</f>
-        <v>49803</v>
+        <v>49807</v>
       </c>
       <c r="M77" s="119"/>
       <c r="O77" s="162"/>
@@ -7609,7 +7620,7 @@
       <c r="B78" s="107"/>
       <c r="C78" s="107" t="str">
         <f>Swaps!K30</f>
-        <v>obj_0027f#0000</v>
+        <v>obj_00268#0000</v>
       </c>
       <c r="D78" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C78)</f>
@@ -7635,11 +7646,11 @@
       </c>
       <c r="J78" s="109">
         <f>_xll.qlRateHelperEarliestDate($C78,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K78" s="110">
         <f>_xll.qlRateHelperLatestDate($C78,Trigger)</f>
-        <v>50168</v>
+        <v>50171</v>
       </c>
       <c r="M78" s="119"/>
       <c r="O78" s="162"/>
@@ -7649,7 +7660,7 @@
       <c r="B79" s="107"/>
       <c r="C79" s="107" t="str">
         <f>Swaps!K31</f>
-        <v>obj_0024b#0000</v>
+        <v>obj_00243#0000</v>
       </c>
       <c r="D79" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C79)</f>
@@ -7675,11 +7686,11 @@
       </c>
       <c r="J79" s="109">
         <f>_xll.qlRateHelperEarliestDate($C79,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K79" s="110">
         <f>_xll.qlRateHelperLatestDate($C79,Trigger)</f>
-        <v>50535</v>
+        <v>50536</v>
       </c>
       <c r="M79" s="119"/>
       <c r="O79" s="162"/>
@@ -7689,7 +7700,7 @@
       <c r="B80" s="107"/>
       <c r="C80" s="107" t="str">
         <f>Swaps!K32</f>
-        <v>obj_00252#0000</v>
+        <v>obj_0027c#0000</v>
       </c>
       <c r="D80" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C80)</f>
@@ -7715,11 +7726,11 @@
       </c>
       <c r="J80" s="109">
         <f>_xll.qlRateHelperEarliestDate($C80,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K80" s="110">
         <f>_xll.qlRateHelperLatestDate($C80,Trigger)</f>
-        <v>50899</v>
+        <v>50901</v>
       </c>
       <c r="M80" s="119"/>
       <c r="O80" s="162"/>
@@ -7729,7 +7740,7 @@
       <c r="B81" s="107"/>
       <c r="C81" s="107" t="str">
         <f>Swaps!K33</f>
-        <v>obj_00280#0000</v>
+        <v>obj_00260#0000</v>
       </c>
       <c r="D81" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C81)</f>
@@ -7737,7 +7748,7 @@
       </c>
       <c r="E81" s="108">
         <f>_xll.qlRateHelperQuoteValue($C81,Trigger)</f>
-        <v>7.2250000000000005E-3</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="F81" s="108">
         <f>_xll.qlSwapRateHelperSpread($C81,Trigger)</f>
@@ -7755,11 +7766,11 @@
       </c>
       <c r="J81" s="109">
         <f>_xll.qlRateHelperEarliestDate($C81,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K81" s="110">
         <f>_xll.qlRateHelperLatestDate($C81,Trigger)</f>
-        <v>51264</v>
+        <v>51267</v>
       </c>
       <c r="M81" s="119"/>
       <c r="O81" s="162"/>
@@ -7769,7 +7780,7 @@
       <c r="B82" s="107"/>
       <c r="C82" s="107" t="str">
         <f>Swaps!K34</f>
-        <v>obj_0025b#0000</v>
+        <v>obj_00289#0000</v>
       </c>
       <c r="D82" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C82)</f>
@@ -7795,11 +7806,11 @@
       </c>
       <c r="J82" s="109">
         <f>_xll.qlRateHelperEarliestDate($C82,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K82" s="110">
         <f>_xll.qlRateHelperLatestDate($C82,Trigger)</f>
-        <v>51629</v>
+        <v>51634</v>
       </c>
       <c r="M82" s="119"/>
       <c r="O82" s="162"/>
@@ -7809,7 +7820,7 @@
       <c r="B83" s="107"/>
       <c r="C83" s="107" t="str">
         <f>Swaps!K35</f>
-        <v>obj_00264#0000</v>
+        <v>obj_00270#0000</v>
       </c>
       <c r="D83" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C83)</f>
@@ -7835,11 +7846,11 @@
       </c>
       <c r="J83" s="109">
         <f>_xll.qlRateHelperEarliestDate($C83,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K83" s="110">
         <f>_xll.qlRateHelperLatestDate($C83,Trigger)</f>
-        <v>51994</v>
+        <v>51998</v>
       </c>
       <c r="M83" s="119"/>
       <c r="O83" s="162"/>
@@ -7849,7 +7860,7 @@
       <c r="B84" s="107"/>
       <c r="C84" s="107" t="str">
         <f>Swaps!K36</f>
-        <v>obj_00263#0000</v>
+        <v>obj_00287#0000</v>
       </c>
       <c r="D84" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C84)</f>
@@ -7875,11 +7886,11 @@
       </c>
       <c r="J84" s="109">
         <f>_xll.qlRateHelperEarliestDate($C84,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K84" s="110">
         <f>_xll.qlRateHelperLatestDate($C84,Trigger)</f>
-        <v>52359</v>
+        <v>52362</v>
       </c>
       <c r="M84" s="119"/>
       <c r="O84" s="162"/>
@@ -7889,7 +7900,7 @@
       <c r="B85" s="107"/>
       <c r="C85" s="107" t="str">
         <f>Swaps!K37</f>
-        <v>obj_00276#0000</v>
+        <v>obj_0027e#0000</v>
       </c>
       <c r="D85" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C85)</f>
@@ -7915,11 +7926,11 @@
       </c>
       <c r="J85" s="109">
         <f>_xll.qlRateHelperEarliestDate($C85,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K85" s="110">
         <f>_xll.qlRateHelperLatestDate($C85,Trigger)</f>
-        <v>52726</v>
+        <v>52728</v>
       </c>
       <c r="M85" s="119"/>
       <c r="O85" s="162"/>
@@ -7929,7 +7940,7 @@
       <c r="B86" s="107"/>
       <c r="C86" s="107" t="str">
         <f>Swaps!K38</f>
-        <v>obj_00268#0000</v>
+        <v>obj_00285#0000</v>
       </c>
       <c r="D86" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C86)</f>
@@ -7937,7 +7948,7 @@
       </c>
       <c r="E86" s="108">
         <f>_xll.qlRateHelperQuoteValue($C86,Trigger)</f>
-        <v>7.6E-3</v>
+        <v>9.8999999999999991E-3</v>
       </c>
       <c r="F86" s="108">
         <f>_xll.qlSwapRateHelperSpread($C86,Trigger)</f>
@@ -7955,11 +7966,11 @@
       </c>
       <c r="J86" s="109">
         <f>_xll.qlRateHelperEarliestDate($C86,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K86" s="110">
         <f>_xll.qlRateHelperLatestDate($C86,Trigger)</f>
-        <v>53090</v>
+        <v>53093</v>
       </c>
       <c r="M86" s="119"/>
       <c r="O86" s="162"/>
@@ -7969,7 +7980,7 @@
       <c r="B87" s="107"/>
       <c r="C87" s="107" t="str">
         <f>Swaps!K39</f>
-        <v>obj_00258#0000</v>
+        <v>obj_0027f#0000</v>
       </c>
       <c r="D87" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C87)</f>
@@ -7977,7 +7988,7 @@
       </c>
       <c r="E87" s="108">
         <f>_xll.qlRateHelperQuoteValue($C87,Trigger)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F87" s="108">
         <f>_xll.qlSwapRateHelperSpread($C87,Trigger)</f>
@@ -7995,11 +8006,11 @@
       </c>
       <c r="J87" s="109">
         <f>_xll.qlRateHelperEarliestDate($C87,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K87" s="110">
         <f>_xll.qlRateHelperLatestDate($C87,Trigger)</f>
-        <v>54917</v>
+        <v>54919</v>
       </c>
       <c r="M87" s="119"/>
       <c r="O87" s="162"/>
@@ -8009,7 +8020,7 @@
       <c r="B88" s="107"/>
       <c r="C88" s="107" t="str">
         <f>Swaps!K40</f>
-        <v>obj_0025d#0000</v>
+        <v>obj_00278#0000</v>
       </c>
       <c r="D88" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C88)</f>
@@ -8017,7 +8028,7 @@
       </c>
       <c r="E88" s="108">
         <f>_xll.qlRateHelperQuoteValue($C88,Trigger)</f>
-        <v>7.6500000000000014E-3</v>
+        <v>9.9500000000000005E-3</v>
       </c>
       <c r="F88" s="108">
         <f>_xll.qlSwapRateHelperSpread($C88,Trigger)</f>
@@ -8035,11 +8046,11 @@
       </c>
       <c r="J88" s="109">
         <f>_xll.qlRateHelperEarliestDate($C88,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K88" s="110">
         <f>_xll.qlRateHelperLatestDate($C88,Trigger)</f>
-        <v>56744</v>
+        <v>56745</v>
       </c>
       <c r="M88" s="119"/>
       <c r="O88" s="162"/>
@@ -8049,7 +8060,7 @@
       <c r="B89" s="107"/>
       <c r="C89" s="107" t="str">
         <f>Swaps!K41</f>
-        <v>obj_0027a#0000</v>
+        <v>obj_00247#0000</v>
       </c>
       <c r="D89" s="107" t="str">
         <f>_xll.qlRateHelperQuoteName(C89)</f>
@@ -8057,7 +8068,7 @@
       </c>
       <c r="E89" s="108">
         <f>_xll.qlRateHelperQuoteValue($C89,Trigger)</f>
-        <v>7.3000000000000001E-3</v>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="F89" s="108">
         <f>_xll.qlSwapRateHelperSpread($C89,Trigger)</f>
@@ -8075,11 +8086,11 @@
       </c>
       <c r="J89" s="109">
         <f>_xll.qlRateHelperEarliestDate($C89,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K89" s="110">
         <f>_xll.qlRateHelperLatestDate($C89,Trigger)</f>
-        <v>60395</v>
+        <v>60398</v>
       </c>
       <c r="M89" s="119"/>
     </row>
@@ -8088,7 +8099,7 @@
       <c r="B90" s="204"/>
       <c r="C90" s="111" t="str">
         <f>Swaps!K42</f>
-        <v>obj_00286#0000</v>
+        <v>obj_00240#0000</v>
       </c>
       <c r="D90" s="111" t="str">
         <f>_xll.qlRateHelperQuoteName(C90)</f>
@@ -8114,11 +8125,11 @@
       </c>
       <c r="J90" s="114">
         <f>_xll.qlRateHelperEarliestDate($C90,Trigger)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="K90" s="115">
         <f>_xll.qlRateHelperLatestDate($C90,Trigger)</f>
-        <v>64047</v>
+        <v>64052</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8234,8 +8245,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Y126"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -8284,7 +8295,7 @@
       </c>
       <c r="J1" s="68">
         <f t="array" ref="J1:J126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>-7.756497240968694E-3</v>
+        <v>-7.604245877810562E-3</v>
       </c>
       <c r="O1" s="151"/>
     </row>
@@ -8297,15 +8308,15 @@
       </c>
       <c r="D2" s="69" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_0023a</v>
+        <v>obj_00235</v>
       </c>
       <c r="E2" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
-        <v>CHFSND_Quote</v>
+        <v>CHFOND_Quote</v>
       </c>
       <c r="F2" s="70">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>-7.6500000000000005E-3</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="G2" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -8313,14 +8324,14 @@
       </c>
       <c r="H2" s="78">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>42132</v>
+        <v>42131</v>
       </c>
       <c r="I2" s="79">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42135</v>
+        <v>42132</v>
       </c>
       <c r="J2" s="68">
-        <v>-7.756497240968694E-3</v>
+        <v>-7.604245877810562E-3</v>
       </c>
       <c r="M2" s="154"/>
       <c r="O2" s="154"/>
@@ -8336,15 +8347,15 @@
         <v>0</v>
       </c>
       <c r="D3" s="69" t="str">
-        <v>obj_00236</v>
+        <v>obj_00230</v>
       </c>
       <c r="E3" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
-        <v>CHFSWD_Quote</v>
+        <v>CHFTND_Quote</v>
       </c>
       <c r="F3" s="70">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>-8.0800000000000004E-3</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="G3" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -8356,10 +8367,10 @@
       </c>
       <c r="I3" s="79">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42139</v>
+        <v>42135</v>
       </c>
       <c r="J3" s="68">
-        <v>-8.0958950357108827E-3</v>
+        <v>-7.604364699535706E-3</v>
       </c>
       <c r="M3" s="154"/>
       <c r="O3" s="154"/>
@@ -8375,15 +8386,15 @@
         <v>2</v>
       </c>
       <c r="D4" s="69" t="str">
-        <v>obj_00234</v>
+        <v>obj_00237</v>
       </c>
       <c r="E4" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
-        <v>CHF1MD_Quote</v>
+        <v>CHFSND_Quote</v>
       </c>
       <c r="F4" s="70">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>-8.1700000000000002E-3</v>
+        <v>-7.6500000000000005E-3</v>
       </c>
       <c r="G4" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -8391,14 +8402,14 @@
       </c>
       <c r="H4" s="78">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I4" s="79">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42163</v>
+        <v>42136</v>
       </c>
       <c r="J4" s="68">
-        <v>-8.2542728599243123E-3</v>
+        <v>-7.6347582419343807E-3</v>
       </c>
       <c r="M4" s="154"/>
       <c r="V4" s="119"/>
@@ -8413,15 +8424,15 @@
         <v>46</v>
       </c>
       <c r="D5" s="69" t="str">
-        <v>obj_00235</v>
+        <v>obj_00236</v>
       </c>
       <c r="E5" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
-        <v>CHF2MD_Quote</v>
+        <v>CHFSWD_Quote</v>
       </c>
       <c r="F5" s="70">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>-8.09E-3</v>
+        <v>-8.0600000000000012E-3</v>
       </c>
       <c r="G5" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -8429,14 +8440,14 @@
       </c>
       <c r="H5" s="78">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I5" s="79">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42193</v>
+        <v>42142</v>
       </c>
       <c r="J5" s="68">
-        <v>-8.1936551296653889E-3</v>
+        <v>-7.9659593560215975E-3</v>
       </c>
       <c r="M5" s="154"/>
       <c r="V5" s="119"/>
@@ -8452,30 +8463,30 @@
         <v/>
       </c>
       <c r="D6" s="69" t="str">
-        <v>obj_00269</v>
+        <v>obj_00238</v>
       </c>
       <c r="E6" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
-        <v>CHFFUT3MM5_Quote</v>
+        <v>CHF1MD_Quote</v>
       </c>
       <c r="F6" s="70">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="70">
+        <v>-8.1700000000000002E-3</v>
+      </c>
+      <c r="G6" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
-        <v>0</v>
+        <v>--</v>
       </c>
       <c r="H6" s="78">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>42172</v>
+        <v>42135</v>
       </c>
       <c r="I6" s="79">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42264</v>
+        <v>42166</v>
       </c>
       <c r="J6" s="68">
-        <v>0.61731424240852228</v>
+        <v>-8.2084419626768292E-3</v>
       </c>
       <c r="M6" s="154"/>
       <c r="V6" s="119"/>
@@ -8484,30 +8495,30 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D7" s="69" t="str">
-        <v>obj_00287</v>
+        <v>obj_0023a</v>
       </c>
       <c r="E7" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
-        <v>CHFFUT3MU5_Quote</v>
+        <v>CHF2MD_Quote</v>
       </c>
       <c r="F7" s="70">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="70">
+        <v>-8.09E-3</v>
+      </c>
+      <c r="G7" s="70" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
-        <v>0</v>
+        <v>--</v>
       </c>
       <c r="H7" s="78">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>42263</v>
+        <v>42135</v>
       </c>
       <c r="I7" s="79">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42354</v>
+        <v>42198</v>
       </c>
       <c r="J7" s="68">
-        <v>0.72852087329427939</v>
+        <v>-8.172124596040253E-3</v>
       </c>
       <c r="M7" s="154"/>
       <c r="V7" s="119"/>
@@ -8516,15 +8527,15 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D8" s="69" t="str">
-        <v>obj_0026d</v>
+        <v>obj_00252</v>
       </c>
       <c r="E8" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
-        <v>CHFFUT3MZ5_Quote</v>
+        <v>CHFFUT3MM5_Quote</v>
       </c>
       <c r="F8" s="70">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1</v>
+        <v>-8.0500000000001126E-3</v>
       </c>
       <c r="G8" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -8532,14 +8543,14 @@
       </c>
       <c r="H8" s="78">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>42354</v>
+        <v>42172</v>
       </c>
       <c r="I8" s="79">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42445</v>
+        <v>42264</v>
       </c>
       <c r="J8" s="68">
-        <v>0.77919454938758481</v>
+        <v>-8.179898289848532E-3</v>
       </c>
       <c r="M8" s="154"/>
       <c r="O8" s="154"/>
@@ -8549,15 +8560,15 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D9" s="69" t="str">
-        <v>obj_00289</v>
+        <v>obj_0026e</v>
       </c>
       <c r="E9" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
-        <v>CHFFUT3MH6_Quote</v>
+        <v>CHFFUT3MU5_Quote</v>
       </c>
       <c r="F9" s="70">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1</v>
+        <v>-8.0500000000001126E-3</v>
       </c>
       <c r="G9" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -8565,14 +8576,14 @@
       </c>
       <c r="H9" s="78">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42445</v>
+        <v>42263</v>
       </c>
       <c r="I9" s="79">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42537</v>
+        <v>42354</v>
       </c>
       <c r="J9" s="68">
-        <v>0.80715554598660133</v>
+        <v>-8.1758386974023316E-3</v>
       </c>
       <c r="M9" s="154"/>
       <c r="O9" s="154"/>
@@ -8582,15 +8593,15 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D10" s="69" t="str">
-        <v>obj_0025f</v>
+        <v>obj_0023b</v>
       </c>
       <c r="E10" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
-        <v>CHFFUT3MM6_Quote</v>
+        <v>CHFFUT3MZ5_Quote</v>
       </c>
       <c r="F10" s="70">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>1</v>
+        <v>-7.6499999999999346E-3</v>
       </c>
       <c r="G10" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -8598,14 +8609,14 @@
       </c>
       <c r="H10" s="78">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42536</v>
+        <v>42354</v>
       </c>
       <c r="I10" s="79">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42628</v>
+        <v>42445</v>
       </c>
       <c r="J10" s="68">
-        <v>0.82459394123761198</v>
+        <v>-8.0564143282969396E-3</v>
       </c>
       <c r="M10" s="154"/>
       <c r="O10" s="154"/>
@@ -8615,15 +8626,15 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D11" s="69" t="str">
-        <v>obj_00247</v>
+        <v>obj_0025a</v>
       </c>
       <c r="E11" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
-        <v>CHFFUT3MU6_Quote</v>
+        <v>CHFFUT3MH6_Quote</v>
       </c>
       <c r="F11" s="70">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>1</v>
+        <v>-7.1000000000001062E-3</v>
       </c>
       <c r="G11" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -8631,14 +8642,14 @@
       </c>
       <c r="H11" s="78">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42634</v>
+        <v>42445</v>
       </c>
       <c r="I11" s="79">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42725</v>
+        <v>42537</v>
       </c>
       <c r="J11" s="68">
-        <v>0.83739855629855786</v>
+        <v>-7.863516938817856E-3</v>
       </c>
       <c r="M11" s="154"/>
       <c r="O11" s="154"/>
@@ -8648,15 +8659,15 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D12" s="69" t="str">
-        <v>obj_0024c</v>
+        <v>obj_0026d</v>
       </c>
       <c r="E12" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
-        <v>CHFAB6L2Y_Quote</v>
+        <v>CHFFUT3MM6_Quote</v>
       </c>
       <c r="F12" s="70">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>-6.4000000000000003E-3</v>
+        <v>-6.4500000000000668E-3</v>
       </c>
       <c r="G12" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -8664,14 +8675,14 @@
       </c>
       <c r="H12" s="78">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42132</v>
+        <v>42536</v>
       </c>
       <c r="I12" s="79">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42863</v>
+        <v>42628</v>
       </c>
       <c r="J12" s="68">
-        <v>-4.637037881941114E-3</v>
+        <v>-7.6211500871597249E-3</v>
       </c>
       <c r="M12" s="154"/>
       <c r="O12" s="154"/>
@@ -8681,15 +8692,15 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D13" s="69" t="str">
-        <v>obj_0026c</v>
+        <v>obj_0026a</v>
       </c>
       <c r="E13" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
-        <v>CHFAB6L3Y_Quote</v>
+        <v>CHFFUT3MU6_Quote</v>
       </c>
       <c r="F13" s="70">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>-5.1999999999999998E-3</v>
+        <v>-5.8000000000000274E-3</v>
       </c>
       <c r="G13" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -8697,14 +8708,14 @@
       </c>
       <c r="H13" s="78">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42132</v>
+        <v>42634</v>
       </c>
       <c r="I13" s="79">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>43228</v>
+        <v>42725</v>
       </c>
       <c r="J13" s="68">
-        <v>-4.2530882791292461E-3</v>
+        <v>-7.3404515615824312E-3</v>
       </c>
       <c r="M13" s="154"/>
       <c r="O13" s="154"/>
@@ -8714,15 +8725,15 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D14" s="69" t="str">
-        <v>obj_00275</v>
+        <v>obj_00264</v>
       </c>
       <c r="E14" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D14)</f>
-        <v>CHFAB6L4Y_Quote</v>
+        <v>CHFAB6L2Y_Quote</v>
       </c>
       <c r="F14" s="70">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>-3.7499999999999999E-3</v>
+        <v>-5.9000000000000007E-3</v>
       </c>
       <c r="G14" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -8730,14 +8741,14 @@
       </c>
       <c r="H14" s="78">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I14" s="79">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>43593</v>
+        <v>42866</v>
       </c>
       <c r="J14" s="68">
-        <v>-3.2462847963328134E-3</v>
+        <v>-5.9246066469831838E-3</v>
       </c>
       <c r="M14" s="154"/>
       <c r="O14" s="154"/>
@@ -8747,15 +8758,15 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D15" s="69" t="str">
-        <v>obj_00265</v>
+        <v>obj_00273</v>
       </c>
       <c r="E15" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D15)</f>
-        <v>CHFAB6L5Y_Quote</v>
+        <v>CHFAB6L3Y_Quote</v>
       </c>
       <c r="F15" s="70">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>-2.2750000000000001E-3</v>
+        <v>-4.5750000000000001E-3</v>
       </c>
       <c r="G15" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -8763,14 +8774,14 @@
       </c>
       <c r="H15" s="78">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I15" s="79">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>43959</v>
+        <v>43231</v>
       </c>
       <c r="J15" s="68">
-        <v>-2.0371743385366602E-3</v>
+        <v>-4.6014887333829966E-3</v>
       </c>
       <c r="M15" s="154"/>
       <c r="O15" s="154"/>
@@ -8780,15 +8791,15 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D16" s="69" t="str">
-        <v>obj_00277</v>
+        <v>obj_00245</v>
       </c>
       <c r="E16" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D16)</f>
-        <v>CHFAB6L6Y_Quote</v>
+        <v>CHFAB6L4Y_Quote</v>
       </c>
       <c r="F16" s="70">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>-8.7499999999999991E-4</v>
+        <v>-2.9500000000000004E-3</v>
       </c>
       <c r="G16" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -8796,14 +8807,14 @@
       </c>
       <c r="H16" s="78">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I16" s="79">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>44326</v>
+        <v>43598</v>
       </c>
       <c r="J16" s="68">
-        <v>-8.0527243003075232E-4</v>
+        <v>-2.9767310000426051E-3</v>
       </c>
       <c r="M16" s="154"/>
       <c r="V16" s="119"/>
@@ -8812,15 +8823,15 @@
     </row>
     <row r="17" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D17" s="69" t="str">
-        <v>obj_00250</v>
+        <v>obj_00284</v>
       </c>
       <c r="E17" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D17)</f>
-        <v>CHFAB6L7Y_Quote</v>
+        <v>CHFAB6L5Y_Quote</v>
       </c>
       <c r="F17" s="70">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>3.4999999999999994E-4</v>
+        <v>-1.2999999999999999E-3</v>
       </c>
       <c r="G17" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -8828,14 +8839,14 @@
       </c>
       <c r="H17" s="78">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I17" s="79">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>44690</v>
+        <v>43962</v>
       </c>
       <c r="J17" s="68">
-        <v>3.1850384689562588E-4</v>
+        <v>-1.3216359979824667E-3</v>
       </c>
       <c r="M17" s="154"/>
       <c r="O17" s="154"/>
@@ -8846,15 +8857,15 @@
     </row>
     <row r="18" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D18" s="69" t="str">
-        <v>obj_0027b</v>
+        <v>obj_00282</v>
       </c>
       <c r="E18" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D18)</f>
-        <v>CHFAB6L8Y_Quote</v>
+        <v>CHFAB6L6Y_Quote</v>
       </c>
       <c r="F18" s="70">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.4000000000000002E-3</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="G18" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -8862,14 +8873,14 @@
       </c>
       <c r="H18" s="78">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I18" s="79">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>45054</v>
+        <v>44327</v>
       </c>
       <c r="J18" s="68">
-        <v>1.3093887386317171E-3</v>
+        <v>2.3776813316206622E-4</v>
       </c>
       <c r="M18" s="154"/>
       <c r="O18" s="154"/>
@@ -8880,15 +8891,15 @@
     </row>
     <row r="19" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D19" s="69" t="str">
-        <v>obj_00256</v>
+        <v>obj_00248</v>
       </c>
       <c r="E19" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D19)</f>
-        <v>CHFAB6L9Y_Quote</v>
+        <v>CHFAB6L7Y_Quote</v>
       </c>
       <c r="F19" s="70">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>2.2750000000000001E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G19" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -8896,14 +8907,14 @@
       </c>
       <c r="H19" s="78">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I19" s="79">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>45420</v>
+        <v>44692</v>
       </c>
       <c r="J19" s="68">
-        <v>2.1524046972604058E-3</v>
+        <v>1.6025057409084016E-3</v>
       </c>
       <c r="M19" s="154"/>
       <c r="O19" s="154"/>
@@ -8914,15 +8925,15 @@
     </row>
     <row r="20" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D20" s="69" t="str">
-        <v>obj_0023d</v>
+        <v>obj_00274</v>
       </c>
       <c r="E20" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D20)</f>
-        <v>CHFAB6L10Y_Quote</v>
+        <v>CHFAB6L8Y_Quote</v>
       </c>
       <c r="F20" s="70">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>3.0000000000000005E-3</v>
+        <v>2.7750000000000001E-3</v>
       </c>
       <c r="G20" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -8930,14 +8941,14 @@
       </c>
       <c r="H20" s="78">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I20" s="79">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>45785</v>
+        <v>45057</v>
       </c>
       <c r="J20" s="68">
-        <v>2.8634021355880097E-3</v>
+        <v>2.79624742922572E-3</v>
       </c>
       <c r="M20" s="154"/>
       <c r="O20" s="154"/>
@@ -8948,15 +8959,15 @@
     </row>
     <row r="21" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D21" s="69" t="str">
-        <v>obj_00242</v>
+        <v>obj_0025d</v>
       </c>
       <c r="E21" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D21)</f>
-        <v>CHFAB6L11Y_Quote</v>
+        <v>CHFAB6L9Y_Quote</v>
       </c>
       <c r="F21" s="70">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>3.5750000000000005E-3</v>
+        <v>3.7499999999999999E-3</v>
       </c>
       <c r="G21" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -8964,14 +8975,14 @@
       </c>
       <c r="H21" s="78">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I21" s="79">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>46150</v>
+        <v>45425</v>
       </c>
       <c r="J21" s="68">
-        <v>3.4358262398558027E-3</v>
+        <v>3.7903454493869036E-3</v>
       </c>
       <c r="M21" s="154"/>
       <c r="O21" s="154"/>
@@ -8982,15 +8993,15 @@
     </row>
     <row r="22" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D22" s="69" t="str">
-        <v>obj_00282</v>
+        <v>obj_00272</v>
       </c>
       <c r="E22" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D22)</f>
-        <v>CHFAB6L12Y_Quote</v>
+        <v>CHFAB6L10Y_Quote</v>
       </c>
       <c r="F22" s="70">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>4.5500000000000011E-3</v>
       </c>
       <c r="G22" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -8998,14 +9009,14 @@
       </c>
       <c r="H22" s="78">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I22" s="79">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>46517</v>
+        <v>45789</v>
       </c>
       <c r="J22" s="68">
-        <v>3.9638026737529621E-3</v>
+        <v>4.6102495615001063E-3</v>
       </c>
       <c r="M22" s="154"/>
       <c r="O22" s="154"/>
@@ -9016,15 +9027,15 @@
     </row>
     <row r="23" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D23" s="69" t="str">
-        <v>obj_00285</v>
+        <v>obj_00251</v>
       </c>
       <c r="E23" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D23)</f>
-        <v>CHFAB6L15Y_Quote</v>
+        <v>CHFAB6L11Y_Quote</v>
       </c>
       <c r="F23" s="70">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>5.3E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="G23" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -9032,14 +9043,14 @@
       </c>
       <c r="H23" s="78">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I23" s="79">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>47611</v>
+        <v>46153</v>
       </c>
       <c r="J23" s="68">
-        <v>5.191166410214553E-3</v>
+        <v>5.2786639815969082E-3</v>
       </c>
       <c r="M23" s="154"/>
       <c r="O23" s="154"/>
@@ -9049,15 +9060,15 @@
     </row>
     <row r="24" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D24" s="69" t="str">
-        <v>obj_00253</v>
+        <v>obj_0024d</v>
       </c>
       <c r="E24" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D24)</f>
-        <v>CHFAB6L20Y_Quote</v>
+        <v>CHFAB6L12Y_Quote</v>
       </c>
       <c r="F24" s="70">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>6.5000000000000006E-3</v>
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="G24" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -9065,14 +9076,14 @@
       </c>
       <c r="H24" s="78">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I24" s="79">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>49437</v>
+        <v>46518</v>
       </c>
       <c r="J24" s="68">
-        <v>6.4518054341542678E-3</v>
+        <v>5.8460152988804217E-3</v>
       </c>
       <c r="M24" s="154"/>
       <c r="O24" s="154"/>
@@ -9082,15 +9093,15 @@
     </row>
     <row r="25" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D25" s="69" t="str">
-        <v>obj_00280</v>
+        <v>obj_0027b</v>
       </c>
       <c r="E25" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D25)</f>
-        <v>CHFAB6L25Y_Quote</v>
+        <v>CHFAB6L15Y_Quote</v>
       </c>
       <c r="F25" s="70">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>7.2250000000000005E-3</v>
+        <v>7.0500000000000007E-3</v>
       </c>
       <c r="G25" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -9098,14 +9109,14 @@
       </c>
       <c r="H25" s="78">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I25" s="79">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>51264</v>
+        <v>47616</v>
       </c>
       <c r="J25" s="68">
-        <v>7.2290947412320568E-3</v>
+        <v>7.1951164065095895E-3</v>
       </c>
       <c r="M25" s="154"/>
       <c r="O25" s="154"/>
@@ -9115,15 +9126,15 @@
     </row>
     <row r="26" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D26" s="69" t="str">
-        <v>obj_00268</v>
+        <v>obj_00266</v>
       </c>
       <c r="E26" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D26)</f>
-        <v>CHFAB6L30Y_Quote</v>
+        <v>CHFAB6L20Y_Quote</v>
       </c>
       <c r="F26" s="70">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>7.6E-3</v>
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="G26" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -9131,14 +9142,14 @@
       </c>
       <c r="H26" s="78">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I26" s="79">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>53090</v>
+        <v>49440</v>
       </c>
       <c r="J26" s="68">
-        <v>7.6357209346565678E-3</v>
+        <v>8.4480572586407513E-3</v>
       </c>
       <c r="M26" s="154"/>
       <c r="O26" s="154"/>
@@ -9148,15 +9159,15 @@
     </row>
     <row r="27" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D27" s="69" t="str">
-        <v>obj_00258</v>
+        <v>obj_00260</v>
       </c>
       <c r="E27" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D27)</f>
-        <v>CHFAB6L35Y_Quote</v>
+        <v>CHFAB6L25Y_Quote</v>
       </c>
       <c r="F27" s="70">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>8.9499999999999996E-3</v>
       </c>
       <c r="G27" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -9164,14 +9175,14 @@
       </c>
       <c r="H27" s="78">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I27" s="79">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>54917</v>
+        <v>51267</v>
       </c>
       <c r="J27" s="68">
-        <v>7.7386548826515831E-3</v>
+        <v>9.1810064553431454E-3</v>
       </c>
       <c r="M27" s="154"/>
       <c r="O27" s="154"/>
@@ -9181,15 +9192,15 @@
     </row>
     <row r="28" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D28" s="69" t="str">
-        <v>obj_0025d</v>
+        <v>obj_00285</v>
       </c>
       <c r="E28" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D28)</f>
-        <v>CHFAB6L40Y_Quote</v>
+        <v>CHFAB6L30Y_Quote</v>
       </c>
       <c r="F28" s="70">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>7.6500000000000014E-3</v>
+        <v>9.3250000000000017E-3</v>
       </c>
       <c r="G28" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -9197,14 +9208,14 @@
       </c>
       <c r="H28" s="78">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I28" s="79">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>56744</v>
+        <v>53093</v>
       </c>
       <c r="J28" s="68">
-        <v>7.6721248616938749E-3</v>
+        <v>9.5667641637422109E-3</v>
       </c>
       <c r="M28" s="154"/>
       <c r="O28" s="154"/>
@@ -9214,15 +9225,15 @@
     </row>
     <row r="29" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D29" s="69" t="str">
-        <v>obj_0027a</v>
+        <v>obj_0027f</v>
       </c>
       <c r="E29" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D29)</f>
-        <v>CHFAB6L50Y_Quote</v>
+        <v>CHFAB6L35Y_Quote</v>
       </c>
       <c r="F29" s="70">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>7.3000000000000001E-3</v>
+        <v>9.4250000000000011E-3</v>
       </c>
       <c r="G29" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -9230,14 +9241,14 @@
       </c>
       <c r="H29" s="78">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>42132</v>
+        <v>42135</v>
       </c>
       <c r="I29" s="79">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>60395</v>
+        <v>54919</v>
       </c>
       <c r="J29" s="68">
-        <v>7.2533850281748065E-3</v>
+        <v>9.6435905033565063E-3</v>
       </c>
       <c r="M29" s="154"/>
       <c r="O29" s="154"/>
@@ -9245,31 +9256,31 @@
       <c r="Y29" s="163"/>
     </row>
     <row r="30" spans="4:25" x14ac:dyDescent="0.2">
-      <c r="D30" s="69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" s="69" t="e">
+      <c r="D30" s="69" t="str">
+        <v>obj_00278</v>
+      </c>
+      <c r="E30" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F30" s="70" t="e">
+        <v>CHFAB6L40Y_Quote</v>
+      </c>
+      <c r="F30" s="70">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" s="70" t="str">
+        <v>9.3749999999999997E-3</v>
+      </c>
+      <c r="G30" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
-        <v>--</v>
-      </c>
-      <c r="H30" s="78" t="e">
+        <v>0</v>
+      </c>
+      <c r="H30" s="78">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="79" t="e">
+        <v>42135</v>
+      </c>
+      <c r="I30" s="79">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J30" s="68" t="e">
-        <v>#N/A</v>
+        <v>56745</v>
+      </c>
+      <c r="J30" s="68">
+        <v>9.5496272577922214E-3</v>
       </c>
       <c r="M30" s="154"/>
       <c r="O30" s="154"/>
@@ -9277,31 +9288,31 @@
       <c r="Y30" s="163"/>
     </row>
     <row r="31" spans="4:25" x14ac:dyDescent="0.2">
-      <c r="D31" s="69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" s="69" t="e">
+      <c r="D31" s="69" t="str">
+        <v>obj_00247</v>
+      </c>
+      <c r="E31" s="69" t="str">
         <f>_xll.qlRateHelperQuoteName(D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F31" s="70" t="e">
+        <v>CHFAB6L50Y_Quote</v>
+      </c>
+      <c r="F31" s="70">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" s="70" t="str">
+        <v>9.025E-3</v>
+      </c>
+      <c r="G31" s="70">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
-        <v>--</v>
-      </c>
-      <c r="H31" s="78" t="e">
+        <v>0</v>
+      </c>
+      <c r="H31" s="78">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="79" t="e">
+        <v>42135</v>
+      </c>
+      <c r="I31" s="79">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J31" s="68" t="e">
-        <v>#N/A</v>
+        <v>60398</v>
+      </c>
+      <c r="J31" s="68">
+        <v>9.0752036881841247E-3</v>
       </c>
       <c r="M31" s="154"/>
       <c r="O31" s="154"/>
@@ -12132,7 +12143,7 @@
       </c>
       <c r="C3" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B3,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0022b#0000</v>
+        <v>obj_0022f#0004</v>
       </c>
       <c r="D3" s="197" t="str">
         <f t="shared" ref="D3:D11" si="0">UPPER(Currency)&amp;B3&amp;"D"&amp;QuoteSuffix</f>
@@ -12140,7 +12151,7 @@
       </c>
       <c r="E3" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00233#0000</v>
+        <v>obj_00235#0004</v>
       </c>
       <c r="F3" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -12155,7 +12166,7 @@
       </c>
       <c r="C4" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00229#0000</v>
+        <v>obj_0022a#0004</v>
       </c>
       <c r="D4" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12163,7 +12174,7 @@
       </c>
       <c r="E4" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_0022c#0000</v>
+        <v>obj_00230#0004</v>
       </c>
       <c r="F4" s="140"/>
       <c r="G4" s="192"/>
@@ -12175,7 +12186,7 @@
       </c>
       <c r="C5" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B5,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00230#0000</v>
+        <v>obj_00229#0004</v>
       </c>
       <c r="D5" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12183,7 +12194,7 @@
       </c>
       <c r="E5" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_0023a#0000</v>
+        <v>obj_00237#0004</v>
       </c>
       <c r="F5" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -12198,7 +12209,7 @@
       </c>
       <c r="C6" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0022f#0000</v>
+        <v>obj_00228#0004</v>
       </c>
       <c r="D6" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12206,7 +12217,7 @@
       </c>
       <c r="E6" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D6,C6,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00236#0000</v>
+        <v>obj_00236#0004</v>
       </c>
       <c r="F6" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -12221,7 +12232,7 @@
       </c>
       <c r="C7" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0022e#0000</v>
+        <v>obj_00227#0004</v>
       </c>
       <c r="D7" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12229,7 +12240,7 @@
       </c>
       <c r="E7" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D7,C7,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00234#0000</v>
+        <v>obj_00238#0004</v>
       </c>
       <c r="F7" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -12244,7 +12255,7 @@
       </c>
       <c r="C8" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00228#0000</v>
+        <v>obj_0022d#0004</v>
       </c>
       <c r="D8" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12252,7 +12263,7 @@
       </c>
       <c r="E8" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00235#0000</v>
+        <v>obj_0023a#0004</v>
       </c>
       <c r="F8" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -12267,7 +12278,7 @@
       </c>
       <c r="C9" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0022d#0000</v>
+        <v>obj_0022b#0004</v>
       </c>
       <c r="D9" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12275,7 +12286,7 @@
       </c>
       <c r="E9" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00237#0000</v>
+        <v>obj_00239#0004</v>
       </c>
       <c r="F9" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -12290,7 +12301,7 @@
       </c>
       <c r="C10" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00227#0000</v>
+        <v>obj_0022c#0004</v>
       </c>
       <c r="D10" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12298,7 +12309,7 @@
       </c>
       <c r="E10" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00238#0000</v>
+        <v>obj_00233#0004</v>
       </c>
       <c r="F10" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -12313,7 +12324,7 @@
       </c>
       <c r="C11" s="197" t="str">
         <f>_xll.qlLibor(,Currency,B11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0022a#0000</v>
+        <v>obj_0022e#0004</v>
       </c>
       <c r="D11" s="197" t="str">
         <f t="shared" si="0"/>
@@ -12321,7 +12332,7 @@
       </c>
       <c r="E11" s="197" t="str">
         <f>_xll.qlDepositRateHelper(,D11,C11,Permanent,Trigger,FileOverwrite)</f>
-        <v>obj_00239#0000</v>
+        <v>obj_00234#0004</v>
       </c>
       <c r="F11" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -12438,7 +12449,7 @@
       </c>
       <c r="H3" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0023b#0000</v>
+        <v>obj_00279#0000</v>
       </c>
       <c r="I3" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -12475,7 +12486,7 @@
       </c>
       <c r="H4" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00269#0000</v>
+        <v>obj_00252#0000</v>
       </c>
       <c r="I4" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -12512,7 +12523,7 @@
       </c>
       <c r="H5" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026a#0000</v>
+        <v>obj_0024f#0000</v>
       </c>
       <c r="I5" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -12546,7 +12557,7 @@
       </c>
       <c r="H6" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00248#0000</v>
+        <v>obj_00288#0000</v>
       </c>
       <c r="I6" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -12580,7 +12591,7 @@
       </c>
       <c r="H7" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00287#0000</v>
+        <v>obj_0026e#0000</v>
       </c>
       <c r="I7" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -12614,7 +12625,7 @@
       </c>
       <c r="H8" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00243#0000</v>
+        <v>obj_00276#0000</v>
       </c>
       <c r="I8" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -12648,7 +12659,7 @@
       </c>
       <c r="H9" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00260#0000</v>
+        <v>obj_00263#0000</v>
       </c>
       <c r="I9" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -12682,7 +12693,7 @@
       </c>
       <c r="H10" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026d#0000</v>
+        <v>obj_0023b#0000</v>
       </c>
       <c r="I10" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -12716,7 +12727,7 @@
       </c>
       <c r="H11" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00259#0000</v>
+        <v>obj_00242#0000</v>
       </c>
       <c r="I11" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -12750,7 +12761,7 @@
       </c>
       <c r="H12" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00245#0000</v>
+        <v>obj_0025e#0000</v>
       </c>
       <c r="I12" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -12784,7 +12795,7 @@
       </c>
       <c r="H13" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00289#0000</v>
+        <v>obj_0025a#0000</v>
       </c>
       <c r="I13" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -12818,7 +12829,7 @@
       </c>
       <c r="H14" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027e#0000</v>
+        <v>obj_00265#0000</v>
       </c>
       <c r="I14" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H14)</f>
@@ -12852,7 +12863,7 @@
       </c>
       <c r="H15" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025f#0000</v>
+        <v>obj_0026d#0000</v>
       </c>
       <c r="I15" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H15)</f>
@@ -12886,7 +12897,7 @@
       </c>
       <c r="H16" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00247#0000</v>
+        <v>obj_0026a#0000</v>
       </c>
       <c r="I16" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H16)</f>
@@ -12920,7 +12931,7 @@
       </c>
       <c r="H17" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00249#0000</v>
+        <v>obj_0023f#0000</v>
       </c>
       <c r="I17" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H17)</f>
@@ -12954,7 +12965,7 @@
       </c>
       <c r="H18" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027d#0000</v>
+        <v>obj_00281#0000</v>
       </c>
       <c r="I18" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H18)</f>
@@ -12988,7 +12999,7 @@
       </c>
       <c r="H19" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00278#0000</v>
+        <v>obj_0024a#0000</v>
       </c>
       <c r="I19" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H19)</f>
@@ -13022,7 +13033,7 @@
       </c>
       <c r="H20" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00283#0000</v>
+        <v>obj_00277#0000</v>
       </c>
       <c r="I20" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H20)</f>
@@ -13056,7 +13067,7 @@
       </c>
       <c r="H21" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00254#0000</v>
+        <v>obj_00262#0000</v>
       </c>
       <c r="I21" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H21)</f>
@@ -13090,7 +13101,7 @@
       </c>
       <c r="H22" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025e#0000</v>
+        <v>obj_00267#0000</v>
       </c>
       <c r="I22" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H22)</f>
@@ -13124,7 +13135,7 @@
       </c>
       <c r="H23" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026e#0000</v>
+        <v>obj_00259#0000</v>
       </c>
       <c r="I23" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H23)</f>
@@ -13158,7 +13169,7 @@
       </c>
       <c r="H24" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00240#0000</v>
+        <v>obj_00250#0000</v>
       </c>
       <c r="I24" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H24)</f>
@@ -13192,7 +13203,7 @@
       </c>
       <c r="H25" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00257#0000</v>
+        <v>obj_00246#0000</v>
       </c>
       <c r="I25" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H25)</f>
@@ -13226,7 +13237,7 @@
       </c>
       <c r="H26" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024a#0000</v>
+        <v>obj_0027a#0000</v>
       </c>
       <c r="I26" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H26)</f>
@@ -13260,7 +13271,7 @@
       </c>
       <c r="H27" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00279#0000</v>
+        <v>obj_0026c#0000</v>
       </c>
       <c r="I27" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H27)</f>
@@ -13294,7 +13305,7 @@
       </c>
       <c r="H28" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00273#0000</v>
+        <v>obj_0023e#0000</v>
       </c>
       <c r="I28" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H28)</f>
@@ -13328,7 +13339,7 @@
       </c>
       <c r="H29" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025c#0000</v>
+        <v>obj_00271#0000</v>
       </c>
       <c r="I29" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H29)</f>
@@ -13362,7 +13373,7 @@
       </c>
       <c r="H30" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00251#0000</v>
+        <v>obj_0025b#0000</v>
       </c>
       <c r="I30" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H30)</f>
@@ -13396,7 +13407,7 @@
       </c>
       <c r="H31" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00271#0000</v>
+        <v>obj_00256#0000</v>
       </c>
       <c r="I31" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H31)</f>
@@ -13430,7 +13441,7 @@
       </c>
       <c r="H32" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00262#0000</v>
+        <v>obj_00269#0000</v>
       </c>
       <c r="I32" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H32)</f>
@@ -13464,7 +13475,7 @@
       </c>
       <c r="H33" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024e#0000</v>
+        <v>obj_00258#0000</v>
       </c>
       <c r="I33" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H33)</f>
@@ -13498,7 +13509,7 @@
       </c>
       <c r="H34" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0023e#0000</v>
+        <v>obj_00286#0000</v>
       </c>
       <c r="I34" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H34)</f>
@@ -13532,7 +13543,7 @@
       </c>
       <c r="H35" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0023c#0000</v>
+        <v>obj_00249#0000</v>
       </c>
       <c r="I35" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H35)</f>
@@ -13566,7 +13577,7 @@
       </c>
       <c r="H36" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00272#0000</v>
+        <v>obj_0026f#0000</v>
       </c>
       <c r="I36" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H36)</f>
@@ -13600,7 +13611,7 @@
       </c>
       <c r="H37" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00266#0000</v>
+        <v>obj_0026b#0000</v>
       </c>
       <c r="I37" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H37)</f>
@@ -13634,7 +13645,7 @@
       </c>
       <c r="H38" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024d#0000</v>
+        <v>obj_00255#0000</v>
       </c>
       <c r="I38" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H38)</f>
@@ -13668,7 +13679,7 @@
       </c>
       <c r="H39" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00270#0000</v>
+        <v>obj_00241#0000</v>
       </c>
       <c r="I39" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H39)</f>
@@ -13702,7 +13713,7 @@
       </c>
       <c r="H40" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025a#0000</v>
+        <v>obj_0024c#0000</v>
       </c>
       <c r="I40" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H40)</f>
@@ -13735,7 +13746,7 @@
       </c>
       <c r="H41" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00267#0000</v>
+        <v>obj_0027d#0000</v>
       </c>
       <c r="I41" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H41)</f>
@@ -13768,7 +13779,7 @@
       </c>
       <c r="H42" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00246#0000</v>
+        <v>obj_00253#0000</v>
       </c>
       <c r="I42" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H42)</f>
@@ -13801,7 +13812,7 @@
       </c>
       <c r="H43" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00281#0000</v>
+        <v>obj_0025c#0000</v>
       </c>
       <c r="I43" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H43)</f>
@@ -13834,7 +13845,7 @@
       </c>
       <c r="H44" s="131" t="str">
         <f>_xll.qlFuturesRateHelper(,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00244#0000</v>
+        <v>obj_0023d#0000</v>
       </c>
       <c r="I44" s="49" t="str">
         <f>_xll.ohRangeRetrieveError(H44)</f>
@@ -14060,7 +14071,7 @@
       </c>
       <c r="K6" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$3,$I6,B6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00241#0000</v>
+        <v>obj_00261#0000</v>
       </c>
       <c r="L6" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -14104,7 +14115,7 @@
       </c>
       <c r="K7" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$3,$I7,B7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00284#0000</v>
+        <v>obj_00254#0000</v>
       </c>
       <c r="L7" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -14148,7 +14159,7 @@
       </c>
       <c r="K8" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$3,$I8,B8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00255#0000</v>
+        <v>obj_00257#0000</v>
       </c>
       <c r="L8" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -14192,7 +14203,7 @@
       </c>
       <c r="K9" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$3,$I9,B9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027c#0000</v>
+        <v>obj_0024e#0000</v>
       </c>
       <c r="L9" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -14236,7 +14247,7 @@
       </c>
       <c r="K10" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$3,$I10,B10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024c#0000</v>
+        <v>obj_00264#0000</v>
       </c>
       <c r="L10" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -14280,7 +14291,7 @@
       </c>
       <c r="K11" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$3,$I11,B11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026c#0000</v>
+        <v>obj_00273#0000</v>
       </c>
       <c r="L11" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -14324,7 +14335,7 @@
       </c>
       <c r="K12" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$3,$I12,B12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00275#0000</v>
+        <v>obj_00245#0000</v>
       </c>
       <c r="L12" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -14368,7 +14379,7 @@
       </c>
       <c r="K13" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$3,$I13,B13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00265#0000</v>
+        <v>obj_00284#0000</v>
       </c>
       <c r="L13" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -14411,7 +14422,7 @@
       </c>
       <c r="K14" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$3,$I14,B14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00277#0000</v>
+        <v>obj_00282#0000</v>
       </c>
       <c r="L14" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -14454,7 +14465,7 @@
       </c>
       <c r="K15" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$3,$I15,B15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00250#0000</v>
+        <v>obj_00248#0000</v>
       </c>
       <c r="L15" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -14497,7 +14508,7 @@
       </c>
       <c r="K16" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$3,$I16,B16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027b#0000</v>
+        <v>obj_00274#0000</v>
       </c>
       <c r="L16" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -14540,7 +14551,7 @@
       </c>
       <c r="K17" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$3,$I17,B17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00256#0000</v>
+        <v>obj_0025d#0000</v>
       </c>
       <c r="L17" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -14583,7 +14594,7 @@
       </c>
       <c r="K18" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$3,$I18,B18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0023d#0000</v>
+        <v>obj_00272#0000</v>
       </c>
       <c r="L18" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -14626,7 +14637,7 @@
       </c>
       <c r="K19" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$3,$I19,B19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00242#0000</v>
+        <v>obj_00251#0000</v>
       </c>
       <c r="L19" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -14669,7 +14680,7 @@
       </c>
       <c r="K20" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$3,$I20,B20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00282#0000</v>
+        <v>obj_0024d#0000</v>
       </c>
       <c r="L20" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -14712,7 +14723,7 @@
       </c>
       <c r="K21" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$3,$I21,B21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026b#0000</v>
+        <v>obj_00244#0000</v>
       </c>
       <c r="L21" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -14755,7 +14766,7 @@
       </c>
       <c r="K22" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$3,$I22,B22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0023f#0000</v>
+        <v>obj_00280#0000</v>
       </c>
       <c r="L22" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -14798,7 +14809,7 @@
       </c>
       <c r="K23" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$3,$I23,B23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00285#0000</v>
+        <v>obj_0027b#0000</v>
       </c>
       <c r="L23" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -14841,7 +14852,7 @@
       </c>
       <c r="K24" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$3,$I24,B24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024f#0000</v>
+        <v>obj_0023c#0000</v>
       </c>
       <c r="L24" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -14884,7 +14895,7 @@
       </c>
       <c r="K25" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$3,$I25,B25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00261#0000</v>
+        <v>obj_0024b#0000</v>
       </c>
       <c r="L25" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -14927,7 +14938,7 @@
       </c>
       <c r="K26" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$3,$I26,B26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026f#0000</v>
+        <v>obj_0025f#0000</v>
       </c>
       <c r="L26" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -14970,7 +14981,7 @@
       </c>
       <c r="K27" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$3,$I27,B27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00288#0000</v>
+        <v>obj_00283#0000</v>
       </c>
       <c r="L27" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -15013,7 +15024,7 @@
       </c>
       <c r="K28" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$3,$I28,B28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00253#0000</v>
+        <v>obj_00266#0000</v>
       </c>
       <c r="L28" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>
@@ -15056,7 +15067,7 @@
       </c>
       <c r="K29" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J29,$C29,Calendar,$F29,$G29,$H29,$K$3,$I29,B29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00274#0000</v>
+        <v>obj_00275#0000</v>
       </c>
       <c r="L29" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K29)</f>
@@ -15099,7 +15110,7 @@
       </c>
       <c r="K30" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J30,$C30,Calendar,$F30,$G30,$H30,$K$3,$I30,B30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027f#0000</v>
+        <v>obj_00268#0000</v>
       </c>
       <c r="L30" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K30)</f>
@@ -15142,7 +15153,7 @@
       </c>
       <c r="K31" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J31,$C31,Calendar,$F31,$G31,$H31,$K$3,$I31,B31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024b#0000</v>
+        <v>obj_00243#0000</v>
       </c>
       <c r="L31" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K31)</f>
@@ -15185,7 +15196,7 @@
       </c>
       <c r="K32" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J32,$C32,Calendar,$F32,$G32,$H32,$K$3,$I32,B32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00252#0000</v>
+        <v>obj_0027c#0000</v>
       </c>
       <c r="L32" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K32)</f>
@@ -15228,7 +15239,7 @@
       </c>
       <c r="K33" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J33,$C33,Calendar,$F33,$G33,$H33,$K$3,$I33,B33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00280#0000</v>
+        <v>obj_00260#0000</v>
       </c>
       <c r="L33" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K33)</f>
@@ -15271,7 +15282,7 @@
       </c>
       <c r="K34" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J34,$C34,Calendar,$F34,$G34,$H34,$K$3,$I34,B34,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025b#0000</v>
+        <v>obj_00289#0000</v>
       </c>
       <c r="L34" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K34)</f>
@@ -15314,7 +15325,7 @@
       </c>
       <c r="K35" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J35,$C35,Calendar,$F35,$G35,$H35,$K$3,$I35,B35,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00264#0000</v>
+        <v>obj_00270#0000</v>
       </c>
       <c r="L35" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K35)</f>
@@ -15357,7 +15368,7 @@
       </c>
       <c r="K36" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J36,$C36,Calendar,$F36,$G36,$H36,$K$3,$I36,B36,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00263#0000</v>
+        <v>obj_00287#0000</v>
       </c>
       <c r="L36" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K36)</f>
@@ -15400,7 +15411,7 @@
       </c>
       <c r="K37" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J37,$C37,Calendar,$F37,$G37,$H37,$K$3,$I37,B37,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00276#0000</v>
+        <v>obj_0027e#0000</v>
       </c>
       <c r="L37" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K37)</f>
@@ -15443,7 +15454,7 @@
       </c>
       <c r="K38" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J38,$C38,Calendar,$F38,$G38,$H38,$K$3,$I38,B38,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00268#0000</v>
+        <v>obj_00285#0000</v>
       </c>
       <c r="L38" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K38)</f>
@@ -15486,7 +15497,7 @@
       </c>
       <c r="K39" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J39,$C39,Calendar,$F39,$G39,$H39,$K$3,$I39,B39,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00258#0000</v>
+        <v>obj_0027f#0000</v>
       </c>
       <c r="L39" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K39)</f>
@@ -15529,7 +15540,7 @@
       </c>
       <c r="K40" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J40,$C40,Calendar,$F40,$G40,$H40,$K$3,$I40,B40,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025d#0000</v>
+        <v>obj_00278#0000</v>
       </c>
       <c r="L40" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K40)</f>
@@ -15572,7 +15583,7 @@
       </c>
       <c r="K41" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J41,$C41,Calendar,$F41,$G41,$H41,$K$3,$I41,B41,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027a#0000</v>
+        <v>obj_00247#0000</v>
       </c>
       <c r="L41" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K41)</f>
@@ -15615,7 +15626,7 @@
       </c>
       <c r="K42" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$J42,$C42,Calendar,$F42,$G42,$H42,$K$3,$I42,B42,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00286#0000</v>
+        <v>obj_00240#0000</v>
       </c>
       <c r="L42" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(K42)</f>

</xml_diff>